<commit_message>
[POI4] 0.2.0: Now ready to use apache poi 4.1.2.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRest/meta/api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGenerator/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73CC59B-637D-794D-B98E-D0949F0C57C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="460" windowWidth="21420" windowHeight="14880" tabRatio="860" activeTab="1"/>
+    <workbookView xWindow="2560" yWindow="460" windowWidth="21420" windowHeight="14880" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -33,10 +34,18 @@
     <definedName name="必須">config!$D$5:$D$6</definedName>
     <definedName name="必須フラグ">config!$C$5:$C$7</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -46,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="203">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2153,12 +2162,24 @@
     <t>blanco\rest\valueobject</t>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>field_5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>オブジェクト</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SimpleObject</t>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -3029,6 +3050,36 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3069,36 +3120,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -3180,6 +3201,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3636,8 +3660,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J53"/>
@@ -3646,7 +3670,7 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="27" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -3665,7 +3689,7 @@
     <col min="15" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="19">
       <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
@@ -3673,24 +3697,24 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -3699,7 +3723,7 @@
       </c>
       <c r="C6" s="29"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
         <v>88</v>
       </c>
@@ -3709,7 +3733,7 @@
       <c r="C7" s="61"/>
       <c r="D7" s="61"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
         <v>165</v>
       </c>
@@ -3718,7 +3742,7 @@
       </c>
       <c r="C8" s="29"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
         <v>166</v>
       </c>
@@ -3727,7 +3751,7 @@
       </c>
       <c r="C9" s="29"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4">
       <c r="A10" s="104" t="s">
         <v>167</v>
       </c>
@@ -3736,7 +3760,7 @@
       </c>
       <c r="C10" s="29"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4">
       <c r="A11" s="104" t="s">
         <v>168</v>
       </c>
@@ -3745,7 +3769,7 @@
       </c>
       <c r="C11" s="29"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4">
       <c r="A12" s="104" t="s">
         <v>169</v>
       </c>
@@ -3754,7 +3778,7 @@
       </c>
       <c r="C12" s="29"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4">
       <c r="A13" s="104" t="s">
         <v>170</v>
       </c>
@@ -3763,7 +3787,7 @@
       </c>
       <c r="C13" s="29"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4">
       <c r="A14" s="104" t="s">
         <v>171</v>
       </c>
@@ -3772,7 +3796,7 @@
       </c>
       <c r="C14" s="29"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4">
       <c r="A15" s="104" t="s">
         <v>172</v>
       </c>
@@ -3781,14 +3805,14 @@
       </c>
       <c r="C15" s="29"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4">
       <c r="A16" s="104" t="s">
         <v>143</v>
       </c>
       <c r="B16" s="105"/>
       <c r="C16" s="29"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -3797,7 +3821,7 @@
       </c>
       <c r="C17" s="29"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
@@ -3805,7 +3829,7 @@
       <c r="C18" s="61"/>
       <c r="D18" s="61"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10">
       <c r="A19" s="4" t="s">
         <v>106</v>
       </c>
@@ -3815,7 +3839,7 @@
       <c r="C19" s="61"/>
       <c r="D19" s="61"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -3825,70 +3849,70 @@
       <c r="C20" s="61"/>
       <c r="D20" s="61"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10">
       <c r="A21" s="61"/>
       <c r="B21" s="61"/>
       <c r="C21" s="61"/>
       <c r="D21" s="61"/>
     </row>
-    <row r="22" spans="1:10" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="121" t="s">
+    <row r="22" spans="1:10" s="109" customFormat="1">
+      <c r="A22" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="B22" s="122"/>
-      <c r="C22" s="122"/>
-      <c r="D22" s="122"/>
-      <c r="E22" s="122"/>
-      <c r="F22" s="133"/>
+      <c r="B22" s="108"/>
+      <c r="C22" s="108"/>
+      <c r="D22" s="108"/>
+      <c r="E22" s="108"/>
+      <c r="F22" s="119"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="124" t="s">
+    <row r="23" spans="1:10" s="109" customFormat="1">
+      <c r="A23" s="110" t="s">
         <v>191</v>
       </c>
-      <c r="B23" s="125"/>
-      <c r="C23" s="126" t="s">
+      <c r="B23" s="111"/>
+      <c r="C23" s="112" t="s">
         <v>194</v>
       </c>
-      <c r="D23" s="126"/>
-      <c r="E23" s="126"/>
-      <c r="F23" s="134"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="112"/>
+      <c r="F23" s="120"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="127" t="s">
+    <row r="24" spans="1:10" s="109" customFormat="1">
+      <c r="A24" s="113" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="128"/>
-      <c r="C24" s="129" t="s">
+      <c r="B24" s="114"/>
+      <c r="C24" s="115" t="s">
         <v>196</v>
       </c>
-      <c r="D24" s="130"/>
-      <c r="E24" s="131"/>
-      <c r="F24" s="132"/>
-    </row>
-    <row r="25" spans="1:10" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="127" t="s">
+      <c r="D24" s="116"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="118"/>
+    </row>
+    <row r="25" spans="1:10" s="109" customFormat="1">
+      <c r="A25" s="113" t="s">
         <v>193</v>
       </c>
-      <c r="B25" s="128"/>
-      <c r="C25" s="135" t="s">
+      <c r="B25" s="114"/>
+      <c r="C25" s="121" t="s">
         <v>197</v>
       </c>
-      <c r="D25" s="136"/>
-      <c r="E25" s="137"/>
-      <c r="F25" s="132"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="D25" s="122"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="118"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="6"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10">
       <c r="A27" s="4" t="s">
         <v>71</v>
       </c>
@@ -3897,188 +3921,188 @@
       <c r="D27" s="2"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10">
       <c r="A28" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="107" t="s">
+      <c r="B28" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="108"/>
-      <c r="D28" s="109"/>
+      <c r="C28" s="130"/>
+      <c r="D28" s="131"/>
       <c r="E28" s="31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10">
       <c r="A29" s="52"/>
       <c r="B29" s="3"/>
       <c r="C29" s="29"/>
       <c r="D29" s="54"/>
       <c r="E29" s="52"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10">
       <c r="A30" s="52"/>
       <c r="B30" s="3"/>
       <c r="C30" s="29"/>
       <c r="D30" s="54"/>
       <c r="E30" s="52"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10">
       <c r="A31" s="52"/>
       <c r="B31" s="3"/>
       <c r="C31" s="29"/>
       <c r="D31" s="54"/>
       <c r="E31" s="52"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10">
       <c r="A32" s="52"/>
       <c r="B32" s="3"/>
       <c r="C32" s="29"/>
       <c r="D32" s="54"/>
       <c r="E32" s="52"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5">
       <c r="A33" s="52"/>
       <c r="B33" s="3"/>
       <c r="C33" s="29"/>
       <c r="D33" s="54"/>
       <c r="E33" s="52"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5">
       <c r="A34" s="52"/>
       <c r="B34" s="3"/>
       <c r="C34" s="29"/>
       <c r="D34" s="54"/>
       <c r="E34" s="52"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5">
       <c r="A35" s="52"/>
       <c r="B35" s="3"/>
       <c r="C35" s="29"/>
       <c r="D35" s="54"/>
       <c r="E35" s="52"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5">
       <c r="A36" s="52"/>
       <c r="B36" s="3"/>
       <c r="C36" s="29"/>
       <c r="D36" s="54"/>
       <c r="E36" s="52"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5">
       <c r="A37" s="52"/>
       <c r="B37" s="3"/>
       <c r="C37" s="29"/>
       <c r="D37" s="54"/>
       <c r="E37" s="52"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5">
       <c r="A38" s="52"/>
       <c r="B38" s="3"/>
       <c r="C38" s="29"/>
       <c r="D38" s="54"/>
       <c r="E38" s="52"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5">
       <c r="A39" s="52"/>
       <c r="B39" s="3"/>
       <c r="C39" s="29"/>
       <c r="D39" s="54"/>
       <c r="E39" s="52"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5">
       <c r="A40" s="52"/>
       <c r="B40" s="3"/>
       <c r="C40" s="29"/>
       <c r="D40" s="54"/>
       <c r="E40" s="52"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5">
       <c r="A41" s="52"/>
       <c r="B41" s="3"/>
       <c r="C41" s="29"/>
       <c r="D41" s="54"/>
       <c r="E41" s="52"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5">
       <c r="A42" s="52"/>
       <c r="B42" s="3"/>
       <c r="C42" s="29"/>
       <c r="D42" s="54"/>
       <c r="E42" s="52"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5">
       <c r="A43" s="52"/>
       <c r="B43" s="3"/>
       <c r="C43" s="29"/>
       <c r="D43" s="54"/>
       <c r="E43" s="52"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5">
       <c r="A44" s="52"/>
       <c r="B44" s="3"/>
       <c r="C44" s="29"/>
       <c r="D44" s="54"/>
       <c r="E44" s="52"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5">
       <c r="A45" s="52"/>
       <c r="B45" s="3"/>
       <c r="C45" s="29"/>
       <c r="D45" s="54"/>
       <c r="E45" s="52"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5">
       <c r="A46" s="52"/>
       <c r="B46" s="3"/>
       <c r="C46" s="29"/>
       <c r="D46" s="54"/>
       <c r="E46" s="52"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5">
       <c r="A47" s="52"/>
       <c r="B47" s="3"/>
       <c r="C47" s="29"/>
       <c r="D47" s="54"/>
       <c r="E47" s="52"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5">
       <c r="A48" s="52"/>
       <c r="B48" s="3"/>
       <c r="C48" s="29"/>
       <c r="D48" s="54"/>
       <c r="E48" s="52"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5">
       <c r="A49" s="52"/>
       <c r="B49" s="3"/>
       <c r="C49" s="29"/>
       <c r="D49" s="54"/>
       <c r="E49" s="52"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5">
       <c r="A50" s="52"/>
       <c r="B50" s="3"/>
       <c r="C50" s="29"/>
       <c r="D50" s="54"/>
       <c r="E50" s="52"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5">
       <c r="A51" s="52"/>
       <c r="B51" s="3"/>
       <c r="C51" s="29"/>
       <c r="D51" s="54"/>
       <c r="E51" s="52"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5">
       <c r="A52" s="52"/>
       <c r="B52" s="3"/>
       <c r="C52" s="29"/>
       <c r="D52" s="54"/>
       <c r="E52" s="52"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5">
       <c r="A53" s="53"/>
       <c r="B53" s="38"/>
       <c r="C53" s="55"/>
@@ -4098,7 +4122,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>config!$C$5:$C$6</xm:f>
           </x14:formula1>
@@ -4111,17 +4135,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
@@ -4150,7 +4174,7 @@
     <col min="26" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="19">
       <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
@@ -4158,17 +4182,17 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11">
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11">
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -4179,7 +4203,7 @@
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -4192,7 +4216,7 @@
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
         <v>88</v>
       </c>
@@ -4209,7 +4233,7 @@
       <c r="J7" s="61"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -4217,17 +4241,17 @@
       <c r="C8" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="138"/>
+      <c r="D8" s="124"/>
       <c r="E8" s="61"/>
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
         <v>155</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="139" t="s">
+      <c r="C9" s="125" t="s">
         <v>164</v>
       </c>
       <c r="D9" s="55"/>
@@ -4235,7 +4259,7 @@
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11">
       <c r="A10" s="63" t="s">
         <v>156</v>
       </c>
@@ -4245,7 +4269,7 @@
       <c r="E10" s="61"/>
       <c r="G10" s="29"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11">
       <c r="A11" s="63" t="s">
         <v>157</v>
       </c>
@@ -4255,7 +4279,7 @@
       <c r="E11" s="61"/>
       <c r="G11" s="29"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11">
       <c r="A12" s="63" t="s">
         <v>158</v>
       </c>
@@ -4265,7 +4289,7 @@
       <c r="E12" s="61"/>
       <c r="G12" s="29"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11">
       <c r="A13" s="63" t="s">
         <v>159</v>
       </c>
@@ -4275,37 +4299,37 @@
       <c r="E13" s="61"/>
       <c r="G13" s="29"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11">
       <c r="A14" s="63" t="s">
         <v>160</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="139"/>
+      <c r="C14" s="125"/>
       <c r="D14" s="103"/>
       <c r="E14" s="61"/>
       <c r="G14" s="29"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11">
       <c r="A15" s="63" t="s">
         <v>161</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="139"/>
+      <c r="C15" s="125"/>
       <c r="D15" s="103"/>
       <c r="E15" s="61"/>
       <c r="G15" s="29"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11">
       <c r="A16" s="63" t="s">
         <v>162</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="139"/>
+      <c r="C16" s="125"/>
       <c r="D16" s="103"/>
       <c r="E16" s="61"/>
       <c r="G16" s="29"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18">
       <c r="A17" s="63" t="s">
         <v>142</v>
       </c>
@@ -4317,7 +4341,7 @@
       <c r="E17" s="61"/>
       <c r="G17" s="29"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
@@ -4327,7 +4351,7 @@
       <c r="E18" s="61"/>
       <c r="F18" s="61"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18">
       <c r="A19" s="4" t="s">
         <v>106</v>
       </c>
@@ -4339,68 +4363,68 @@
       <c r="E19" s="61"/>
       <c r="F19" s="61"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18">
       <c r="A20" s="6"/>
       <c r="C20" s="29"/>
     </row>
-    <row r="21" spans="1:18" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="121" t="s">
+    <row r="21" spans="1:18" s="109" customFormat="1">
+      <c r="A21" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="122"/>
-      <c r="C21" s="122"/>
-      <c r="D21" s="122"/>
-      <c r="E21" s="122"/>
-      <c r="F21" s="133"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="119"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:18" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="124" t="s">
+    <row r="22" spans="1:18" s="109" customFormat="1">
+      <c r="A22" s="110" t="s">
         <v>191</v>
       </c>
-      <c r="B22" s="125"/>
-      <c r="C22" s="126" t="s">
+      <c r="B22" s="111"/>
+      <c r="C22" s="112" t="s">
         <v>173</v>
       </c>
-      <c r="D22" s="126"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="134"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="120"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:18" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="127" t="s">
+    <row r="23" spans="1:18" s="109" customFormat="1">
+      <c r="A23" s="113" t="s">
         <v>192</v>
       </c>
-      <c r="B23" s="128"/>
-      <c r="C23" s="129" t="s">
+      <c r="B23" s="114"/>
+      <c r="C23" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="D23" s="130"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="132"/>
-    </row>
-    <row r="24" spans="1:18" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="127" t="s">
+      <c r="D23" s="116"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="118"/>
+    </row>
+    <row r="24" spans="1:18" s="109" customFormat="1">
+      <c r="A24" s="113" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="128"/>
-      <c r="C24" s="140" t="s">
+      <c r="B24" s="114"/>
+      <c r="C24" s="126" t="s">
         <v>199</v>
       </c>
-      <c r="D24" s="141"/>
-      <c r="E24" s="142"/>
-      <c r="F24" s="132"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="D24" s="127"/>
+      <c r="E24" s="128"/>
+      <c r="F24" s="118"/>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="6"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18">
       <c r="A26" s="20" t="s">
         <v>10</v>
       </c>
@@ -4422,51 +4446,51 @@
       <c r="Q26" s="41"/>
       <c r="R26" s="41"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A27" s="112" t="s">
+    <row r="27" spans="1:18">
+      <c r="A27" s="134" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="112" t="s">
+      <c r="B27" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="114" t="s">
+      <c r="C27" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="112" t="s">
+      <c r="D27" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="115" t="s">
+      <c r="E27" s="137" t="s">
         <v>174</v>
       </c>
-      <c r="F27" s="112" t="s">
+      <c r="F27" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="112" t="s">
+      <c r="G27" s="134" t="s">
         <v>117</v>
       </c>
-      <c r="H27" s="110" t="s">
+      <c r="H27" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="I27" s="111"/>
-      <c r="J27" s="110" t="s">
+      <c r="I27" s="133"/>
+      <c r="J27" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="111"/>
+      <c r="K27" s="133"/>
       <c r="L27" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="M27" s="112" t="s">
+      <c r="M27" s="134" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A28" s="113"/>
-      <c r="B28" s="113"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="116"/>
-      <c r="F28" s="113"/>
-      <c r="G28" s="113"/>
+    <row r="28" spans="1:18">
+      <c r="A28" s="135"/>
+      <c r="B28" s="135"/>
+      <c r="C28" s="135"/>
+      <c r="D28" s="135"/>
+      <c r="E28" s="138"/>
+      <c r="F28" s="135"/>
+      <c r="G28" s="135"/>
       <c r="H28" s="31" t="s">
         <v>82</v>
       </c>
@@ -4482,9 +4506,9 @@
       <c r="L28" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="M28" s="113"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M28" s="135"/>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="7">
         <v>1</v>
       </c>
@@ -4513,7 +4537,7 @@
       <c r="L29" s="32"/>
       <c r="M29" s="9"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18">
       <c r="A30" s="10">
         <f t="shared" ref="A30:A32" si="0">A29+1</f>
         <v>2</v>
@@ -4541,7 +4565,7 @@
       <c r="L30" s="33"/>
       <c r="M30" s="12"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18">
       <c r="A31" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4565,7 +4589,7 @@
       <c r="L31" s="33"/>
       <c r="M31" s="14"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:18">
       <c r="A32" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4587,11 +4611,19 @@
       <c r="L32" s="33"/>
       <c r="M32" s="14"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A33" s="10"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="27"/>
+    <row r="33" spans="1:13">
+      <c r="A33" s="10">
+        <v>5</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>202</v>
+      </c>
       <c r="E33" s="27"/>
       <c r="F33" s="93"/>
       <c r="G33" s="27"/>
@@ -4602,7 +4634,7 @@
       <c r="L33" s="34"/>
       <c r="M33" s="14"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:13">
       <c r="A34" s="10"/>
       <c r="B34" s="23"/>
       <c r="C34" s="13"/>
@@ -4617,7 +4649,7 @@
       <c r="L34" s="33"/>
       <c r="M34" s="14"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:13">
       <c r="A35" s="10"/>
       <c r="B35" s="23"/>
       <c r="C35" s="13"/>
@@ -4632,7 +4664,7 @@
       <c r="L35" s="33"/>
       <c r="M35" s="14"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:13">
       <c r="A36" s="10"/>
       <c r="B36" s="23"/>
       <c r="C36" s="13"/>
@@ -4647,7 +4679,7 @@
       <c r="L36" s="33"/>
       <c r="M36" s="14"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:13">
       <c r="A37" s="10"/>
       <c r="B37" s="23"/>
       <c r="C37" s="13"/>
@@ -4662,7 +4694,7 @@
       <c r="L37" s="34"/>
       <c r="M37" s="14"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:13">
       <c r="A38" s="10"/>
       <c r="B38" s="23"/>
       <c r="C38" s="13"/>
@@ -4677,7 +4709,7 @@
       <c r="L38" s="33"/>
       <c r="M38" s="14"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:13">
       <c r="A39" s="10"/>
       <c r="B39" s="23"/>
       <c r="C39" s="13"/>
@@ -4692,7 +4724,7 @@
       <c r="L39" s="33"/>
       <c r="M39" s="14"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:13">
       <c r="A40" s="10"/>
       <c r="B40" s="23"/>
       <c r="C40" s="13"/>
@@ -4707,7 +4739,7 @@
       <c r="L40" s="33"/>
       <c r="M40" s="14"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:13">
       <c r="A41" s="10"/>
       <c r="B41" s="23"/>
       <c r="C41" s="13"/>
@@ -4722,7 +4754,7 @@
       <c r="L41" s="33"/>
       <c r="M41" s="14"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:13">
       <c r="A42" s="10"/>
       <c r="B42" s="23"/>
       <c r="C42" s="13"/>
@@ -4737,7 +4769,7 @@
       <c r="L42" s="33"/>
       <c r="M42" s="14"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:13">
       <c r="A43" s="10"/>
       <c r="B43" s="23"/>
       <c r="C43" s="13"/>
@@ -4752,7 +4784,7 @@
       <c r="L43" s="34"/>
       <c r="M43" s="14"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:13">
       <c r="A44" s="10"/>
       <c r="B44" s="23"/>
       <c r="C44" s="13"/>
@@ -4767,7 +4799,7 @@
       <c r="L44" s="33"/>
       <c r="M44" s="14"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:13">
       <c r="A45" s="10"/>
       <c r="B45" s="23"/>
       <c r="C45" s="13"/>
@@ -4782,7 +4814,7 @@
       <c r="L45" s="33"/>
       <c r="M45" s="14"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:13">
       <c r="A46" s="10"/>
       <c r="B46" s="23"/>
       <c r="C46" s="13"/>
@@ -4797,7 +4829,7 @@
       <c r="L46" s="33"/>
       <c r="M46" s="14"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:13">
       <c r="A47" s="10"/>
       <c r="B47" s="23"/>
       <c r="C47" s="13"/>
@@ -4812,7 +4844,7 @@
       <c r="L47" s="33"/>
       <c r="M47" s="14"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:13">
       <c r="A48" s="10"/>
       <c r="B48" s="23"/>
       <c r="C48" s="13"/>
@@ -4827,7 +4859,7 @@
       <c r="L48" s="34"/>
       <c r="M48" s="14"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:13">
       <c r="A49" s="10"/>
       <c r="B49" s="23"/>
       <c r="C49" s="13"/>
@@ -4842,7 +4874,7 @@
       <c r="L49" s="33"/>
       <c r="M49" s="14"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:13">
       <c r="A50" s="10"/>
       <c r="B50" s="23"/>
       <c r="C50" s="13"/>
@@ -4857,7 +4889,7 @@
       <c r="L50" s="33"/>
       <c r="M50" s="14"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:13">
       <c r="A51" s="10"/>
       <c r="B51" s="23"/>
       <c r="C51" s="13"/>
@@ -4872,7 +4904,7 @@
       <c r="L51" s="34"/>
       <c r="M51" s="14"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:13">
       <c r="A52" s="15"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
@@ -4902,12 +4934,12 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>Validate実装パターン</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C19" r:id="rId1" display="http://tempuri.org/sample"/>
+    <hyperlink ref="C19" r:id="rId1" display="http://tempuri.org/sample" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.11811023622047245"/>
   <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="landscape"/>
@@ -4918,19 +4950,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>config!$E$5:$E$8</xm:f>
           </x14:formula1>
           <xm:sqref>C14:C16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>config!$D$5:$D$8</xm:f>
           </x14:formula1>
           <xm:sqref>C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>config!$C$5:$C$6</xm:f>
           </x14:formula1>
@@ -4943,8 +4975,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M45"/>
@@ -4953,7 +4985,7 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
@@ -4982,7 +5014,7 @@
     <col min="26" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="19">
       <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
@@ -4990,17 +5022,17 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11">
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11">
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -5010,7 +5042,7 @@
       <c r="E5" s="61"/>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -5022,7 +5054,7 @@
       <c r="E6" s="61"/>
       <c r="G6" s="29"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
         <v>88</v>
       </c>
@@ -5038,7 +5070,7 @@
       <c r="J7" s="61"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -5050,7 +5082,7 @@
       <c r="E8" s="61"/>
       <c r="G8" s="29"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
         <v>155</v>
       </c>
@@ -5063,7 +5095,7 @@
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11">
       <c r="A10" s="63" t="s">
         <v>142</v>
       </c>
@@ -5074,7 +5106,7 @@
       <c r="D10" s="102"/>
       <c r="E10" s="61"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -5083,7 +5115,7 @@
       <c r="D11" s="37"/>
       <c r="E11" s="61"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
         <v>106</v>
       </c>
@@ -5094,67 +5126,67 @@
       <c r="D12" s="37"/>
       <c r="E12" s="61"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:11" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="121" t="s">
+    <row r="14" spans="1:11" s="109" customFormat="1">
+      <c r="A14" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="B14" s="122"/>
-      <c r="C14" s="122"/>
-      <c r="D14" s="122"/>
-      <c r="E14" s="122"/>
-      <c r="F14" s="133"/>
+      <c r="B14" s="108"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="119"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:11" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="124" t="s">
+    <row r="15" spans="1:11" s="109" customFormat="1">
+      <c r="A15" s="110" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="125"/>
-      <c r="C15" s="126" t="s">
+      <c r="B15" s="111"/>
+      <c r="C15" s="112" t="s">
         <v>173</v>
       </c>
-      <c r="D15" s="126"/>
-      <c r="E15" s="126"/>
-      <c r="F15" s="134"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="120"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:11" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="127" t="s">
+    <row r="16" spans="1:11" s="109" customFormat="1">
+      <c r="A16" s="113" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="128"/>
-      <c r="C16" s="129" t="s">
+      <c r="B16" s="114"/>
+      <c r="C16" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="D16" s="130"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
-    </row>
-    <row r="17" spans="1:13" s="123" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="127" t="s">
+      <c r="D16" s="116"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="118"/>
+    </row>
+    <row r="17" spans="1:13" s="109" customFormat="1">
+      <c r="A17" s="113" t="s">
         <v>193</v>
       </c>
-      <c r="B17" s="128"/>
-      <c r="C17" s="140" t="s">
+      <c r="B17" s="114"/>
+      <c r="C17" s="126" t="s">
         <v>199</v>
       </c>
-      <c r="D17" s="141"/>
-      <c r="E17" s="142"/>
-      <c r="F17" s="132"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="D17" s="127"/>
+      <c r="E17" s="128"/>
+      <c r="F17" s="118"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="6"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:13">
       <c r="A19" s="63" t="s">
         <v>118</v>
       </c>
@@ -5171,53 +5203,53 @@
       <c r="L19" s="64"/>
       <c r="M19" s="65"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A20" s="115" t="s">
+    <row r="20" spans="1:13" ht="15">
+      <c r="A20" s="137" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="115" t="s">
+      <c r="B20" s="137" t="s">
         <v>120</v>
       </c>
       <c r="C20" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="115" t="s">
+      <c r="D20" s="137" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="115" t="s">
+      <c r="E20" s="137" t="s">
         <v>174</v>
       </c>
-      <c r="F20" s="115" t="s">
+      <c r="F20" s="137" t="s">
         <v>139</v>
       </c>
-      <c r="G20" s="115" t="s">
+      <c r="G20" s="137" t="s">
         <v>138</v>
       </c>
-      <c r="H20" s="120" t="s">
+      <c r="H20" s="142" t="s">
         <v>123</v>
       </c>
-      <c r="I20" s="118"/>
-      <c r="J20" s="117" t="s">
+      <c r="I20" s="140"/>
+      <c r="J20" s="139" t="s">
         <v>124</v>
       </c>
-      <c r="K20" s="118"/>
+      <c r="K20" s="140"/>
       <c r="L20" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="M20" s="115" t="s">
+      <c r="M20" s="137" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A21" s="119"/>
-      <c r="B21" s="119"/>
+    <row r="21" spans="1:13" ht="15">
+      <c r="A21" s="141"/>
+      <c r="B21" s="141"/>
       <c r="C21" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="119"/>
-      <c r="E21" s="116"/>
-      <c r="F21" s="119"/>
-      <c r="G21" s="119"/>
+      <c r="D21" s="141"/>
+      <c r="E21" s="138"/>
+      <c r="F21" s="141"/>
+      <c r="G21" s="141"/>
       <c r="H21" s="69" t="s">
         <v>127</v>
       </c>
@@ -5233,9 +5265,9 @@
       <c r="L21" s="70" t="s">
         <v>131</v>
       </c>
-      <c r="M21" s="119"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M21" s="141"/>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="71">
         <v>1</v>
       </c>
@@ -5260,7 +5292,7 @@
       <c r="L22" s="74"/>
       <c r="M22" s="75"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13">
       <c r="A23" s="71">
         <v>2</v>
       </c>
@@ -5283,7 +5315,7 @@
       <c r="L23" s="72"/>
       <c r="M23" s="75"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13">
       <c r="A24" s="71">
         <v>3</v>
       </c>
@@ -5304,7 +5336,7 @@
       <c r="L24" s="72"/>
       <c r="M24" s="78"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13">
       <c r="A25" s="71">
         <v>4</v>
       </c>
@@ -5325,7 +5357,7 @@
       <c r="L25" s="72"/>
       <c r="M25" s="82"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:13">
       <c r="A26" s="71"/>
       <c r="B26" s="79"/>
       <c r="C26" s="80"/>
@@ -5340,7 +5372,7 @@
       <c r="L26" s="74"/>
       <c r="M26" s="82"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:13">
       <c r="A27" s="71"/>
       <c r="B27" s="79"/>
       <c r="C27" s="80"/>
@@ -5355,7 +5387,7 @@
       <c r="L27" s="72"/>
       <c r="M27" s="82"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:13">
       <c r="A28" s="71"/>
       <c r="B28" s="79"/>
       <c r="C28" s="80"/>
@@ -5370,7 +5402,7 @@
       <c r="L28" s="72"/>
       <c r="M28" s="82"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:13">
       <c r="A29" s="71"/>
       <c r="B29" s="79"/>
       <c r="C29" s="80"/>
@@ -5385,7 +5417,7 @@
       <c r="L29" s="72"/>
       <c r="M29" s="82"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:13">
       <c r="A30" s="71"/>
       <c r="B30" s="79"/>
       <c r="C30" s="80"/>
@@ -5400,7 +5432,7 @@
       <c r="L30" s="74"/>
       <c r="M30" s="82"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:13">
       <c r="A31" s="71"/>
       <c r="B31" s="79"/>
       <c r="C31" s="80"/>
@@ -5415,7 +5447,7 @@
       <c r="L31" s="72"/>
       <c r="M31" s="82"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:13">
       <c r="A32" s="71"/>
       <c r="B32" s="79"/>
       <c r="C32" s="80"/>
@@ -5430,7 +5462,7 @@
       <c r="L32" s="72"/>
       <c r="M32" s="82"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:13">
       <c r="A33" s="71"/>
       <c r="B33" s="79"/>
       <c r="C33" s="80"/>
@@ -5445,7 +5477,7 @@
       <c r="L33" s="72"/>
       <c r="M33" s="82"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:13">
       <c r="A34" s="71"/>
       <c r="B34" s="79"/>
       <c r="C34" s="80"/>
@@ -5460,7 +5492,7 @@
       <c r="L34" s="72"/>
       <c r="M34" s="82"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:13">
       <c r="A35" s="71"/>
       <c r="B35" s="79"/>
       <c r="C35" s="80"/>
@@ -5475,7 +5507,7 @@
       <c r="L35" s="72"/>
       <c r="M35" s="82"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:13">
       <c r="A36" s="71"/>
       <c r="B36" s="79"/>
       <c r="C36" s="80"/>
@@ -5490,7 +5522,7 @@
       <c r="L36" s="74"/>
       <c r="M36" s="82"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:13">
       <c r="A37" s="71"/>
       <c r="B37" s="79"/>
       <c r="C37" s="80"/>
@@ -5505,7 +5537,7 @@
       <c r="L37" s="72"/>
       <c r="M37" s="82"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:13">
       <c r="A38" s="71"/>
       <c r="B38" s="79"/>
       <c r="C38" s="80"/>
@@ -5520,7 +5552,7 @@
       <c r="L38" s="72"/>
       <c r="M38" s="82"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:13">
       <c r="A39" s="71"/>
       <c r="B39" s="79"/>
       <c r="C39" s="80"/>
@@ -5535,7 +5567,7 @@
       <c r="L39" s="72"/>
       <c r="M39" s="82"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:13">
       <c r="A40" s="71"/>
       <c r="B40" s="79"/>
       <c r="C40" s="80"/>
@@ -5550,7 +5582,7 @@
       <c r="L40" s="72"/>
       <c r="M40" s="82"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:13">
       <c r="A41" s="71"/>
       <c r="B41" s="79"/>
       <c r="C41" s="80"/>
@@ -5565,7 +5597,7 @@
       <c r="L41" s="74"/>
       <c r="M41" s="82"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:13">
       <c r="A42" s="71"/>
       <c r="B42" s="79"/>
       <c r="C42" s="80"/>
@@ -5580,7 +5612,7 @@
       <c r="L42" s="72"/>
       <c r="M42" s="82"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:13">
       <c r="A43" s="71"/>
       <c r="B43" s="79"/>
       <c r="C43" s="80"/>
@@ -5595,7 +5627,7 @@
       <c r="L43" s="72"/>
       <c r="M43" s="82"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:13">
       <c r="A44" s="71"/>
       <c r="B44" s="79"/>
       <c r="C44" s="80"/>
@@ -5610,7 +5642,7 @@
       <c r="L44" s="74"/>
       <c r="M44" s="82"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:13">
       <c r="A45" s="83"/>
       <c r="B45" s="84"/>
       <c r="C45" s="85"/>
@@ -5639,7 +5671,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>Validate実装パターン</formula1>
     </dataValidation>
   </dataValidations>
@@ -5652,13 +5684,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>config!$D$5:$D$8</xm:f>
           </x14:formula1>
           <xm:sqref>C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>config!$C$5:$C$6</xm:f>
           </x14:formula1>
@@ -5671,8 +5703,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I57"/>
@@ -5681,14 +5713,14 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="42" customWidth="1"/>
     <col min="2" max="2" width="4.5" style="42" customWidth="1"/>
     <col min="3" max="16384" width="8.83203125" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="19">
       <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
@@ -5696,34 +5728,34 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -5731,7 +5763,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>39</v>
@@ -5739,260 +5771,260 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="A16" s="1"/>
       <c r="C16" s="42" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3">
       <c r="B17" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3">
       <c r="C18" s="42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3">
       <c r="B19" s="1"/>
       <c r="C19" s="42" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3">
       <c r="B20" s="1"/>
       <c r="C20" s="42" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3">
       <c r="A23" s="1"/>
       <c r="B23" s="42" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3">
       <c r="A24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3">
       <c r="A25" s="1"/>
       <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3">
       <c r="A26" s="1"/>
       <c r="B26" s="42" t="s">
         <v>50</v>
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3">
       <c r="A27" s="1"/>
       <c r="C27" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3">
       <c r="A28" s="1"/>
       <c r="B28" s="42" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3">
       <c r="C29" s="42" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3">
       <c r="C30" s="42" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3">
       <c r="C31" s="42" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3">
       <c r="C32" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:3">
       <c r="C33" s="42" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:3">
       <c r="C34" s="42" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:3">
       <c r="B35" s="42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:3">
       <c r="C36" s="42" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:3">
       <c r="B37" s="42" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:3">
       <c r="C38" s="42" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:3">
       <c r="B39" s="42" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:3">
       <c r="C40" s="42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:3">
       <c r="C41" s="42" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:3">
       <c r="C42" s="42" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:3">
       <c r="C43" s="42" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:3">
       <c r="B44" s="42" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:3">
       <c r="C45" s="42" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:3">
       <c r="C46" s="42" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:3">
       <c r="B47" s="42" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:3">
       <c r="C48" s="42" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3">
       <c r="C49" s="42" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3">
       <c r="B50" s="42" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3">
       <c r="C51" s="42" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3">
       <c r="C52" s="42" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3">
       <c r="A54" s="42" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3">
       <c r="B55" s="42" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3">
       <c r="C56" s="42" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3">
       <c r="C57" s="42" t="s">
         <v>97</v>
       </c>
@@ -6005,8 +6037,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F34"/>
@@ -6015,7 +6047,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -6026,7 +6058,7 @@
     <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="19">
       <c r="A1" s="18" t="s">
         <v>28</v>
       </c>
@@ -6037,7 +6069,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -6045,7 +6077,7 @@
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6">
       <c r="A4" s="45" t="s">
         <v>4</v>
       </c>
@@ -6062,7 +6094,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6">
       <c r="A5" s="46" t="s">
         <v>6</v>
       </c>
@@ -6077,7 +6109,7 @@
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6">
       <c r="A6" s="48" t="s">
         <v>7</v>
       </c>
@@ -6092,7 +6124,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6">
       <c r="B7" s="50" t="s">
         <v>20</v>
       </c>
@@ -6104,7 +6136,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6">
       <c r="B8" s="50" t="s">
         <v>21</v>
       </c>
@@ -6115,93 +6147,93 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6">
       <c r="B9" s="50" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6">
       <c r="B10" s="50" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6">
       <c r="B11" s="50" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6">
       <c r="B12" s="50" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6">
       <c r="B13" s="50" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6">
       <c r="B14" s="50"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6">
       <c r="B15" s="50"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6">
       <c r="B16" s="50"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2">
       <c r="B17" s="50"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2">
       <c r="B18" s="50"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2">
       <c r="B19" s="50"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2">
       <c r="B20" s="50"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2">
       <c r="B21" s="50"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2">
       <c r="B22" s="50"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2">
       <c r="B23" s="50"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:2">
       <c r="B24" s="50"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:2">
       <c r="B25" s="50"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:2">
       <c r="B26" s="50"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:2">
       <c r="B27" s="50"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:2">
       <c r="B28" s="50"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:2">
       <c r="B29" s="50"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:2">
       <c r="B30" s="50"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:2">
       <c r="B31" s="50"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:2">
       <c r="B32" s="50"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:2">
       <c r="B33" s="50"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:2">
       <c r="B34" s="51"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.2.6: use serviceId for API name instead of telegramProcessId.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGenerator/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C59FBA2-7B7A-5C48-BF75-478F0A3B362A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FC2B0A-0F68-0149-8B59-0CCFA1F64DF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="680" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="680" windowWidth="21420" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -1933,9 +1933,6 @@
     <t>総称型</t>
   </si>
   <si>
-    <t>BlancoApiSample</t>
-  </si>
-  <si>
     <t>blanco.sample</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -2401,6 +2398,10 @@
   </si>
   <si>
     <t>@field:Max(10)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blancoApiSample</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3644,12 +3645,87 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="60" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3659,9 +3735,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3674,12 +3747,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3718,84 +3785,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3819,15 +3808,33 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3838,12 +3845,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4392,8 +4393,8 @@
   </sheetPr>
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4436,204 +4437,204 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="185" t="s">
+      <c r="A5" s="139" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="185"/>
-      <c r="C5" s="185"/>
-      <c r="D5" s="185"/>
-      <c r="E5" s="185"/>
+      <c r="B5" s="139"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="182" t="s">
+      <c r="A6" s="143" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="183"/>
-      <c r="C6" s="184"/>
-      <c r="D6" s="181" t="s">
-        <v>197</v>
-      </c>
-      <c r="E6" s="181"/>
+      <c r="B6" s="144"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="140" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" s="140"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="139" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="185"/>
-      <c r="C7" s="185"/>
-      <c r="D7" s="181" t="s">
-        <v>166</v>
-      </c>
-      <c r="E7" s="181"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="140" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="140"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="185" t="s">
+      <c r="A8" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="185"/>
-      <c r="C8" s="185"/>
-      <c r="D8" s="181" t="s">
-        <v>162</v>
-      </c>
-      <c r="E8" s="181"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="140" t="s">
+        <v>231</v>
+      </c>
+      <c r="E8" s="140"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="185" t="s">
+      <c r="A9" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="185"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="181" t="s">
+      <c r="B9" s="139"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="140" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="181"/>
+      <c r="E9" s="140"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="185" t="s">
+      <c r="A10" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="185"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
+      <c r="B10" s="139"/>
+      <c r="C10" s="139"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="185" t="s">
+      <c r="A11" s="139" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="185"/>
-      <c r="C11" s="185"/>
-      <c r="D11" s="181" t="s">
-        <v>163</v>
-      </c>
-      <c r="E11" s="181"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="140" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" s="140"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="144" t="s">
+      <c r="A12" s="146" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="146"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="141" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="144"/>
-      <c r="C12" s="144"/>
-      <c r="D12" s="165" t="s">
+      <c r="E12" s="141"/>
+      <c r="F12" s="95" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="165"/>
-      <c r="F12" s="95" t="s">
+      <c r="G12" s="54"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="146" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13" s="146"/>
+      <c r="C13" s="146"/>
+      <c r="D13" s="141" t="s">
+        <v>209</v>
+      </c>
+      <c r="E13" s="141"/>
+      <c r="F13" s="95" t="s">
+        <v>210</v>
+      </c>
+      <c r="G13" s="54"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="146" t="s">
         <v>176</v>
       </c>
-      <c r="G12" s="54"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="144" t="s">
-        <v>212</v>
-      </c>
-      <c r="B13" s="144"/>
-      <c r="C13" s="144"/>
-      <c r="D13" s="165" t="s">
-        <v>210</v>
-      </c>
-      <c r="E13" s="165"/>
-      <c r="F13" s="95" t="s">
-        <v>211</v>
-      </c>
-      <c r="G13" s="54"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="144" t="s">
-        <v>177</v>
-      </c>
-      <c r="B14" s="144"/>
-      <c r="C14" s="144"/>
-      <c r="D14" s="164"/>
-      <c r="E14" s="165"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="146"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="141"/>
       <c r="F14" s="54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G14" s="54"/>
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="144" t="s">
-        <v>217</v>
-      </c>
-      <c r="B15" s="144"/>
-      <c r="C15" s="144"/>
-      <c r="D15" s="164" t="s">
-        <v>215</v>
-      </c>
-      <c r="E15" s="165"/>
+      <c r="A15" s="146" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" s="146"/>
+      <c r="C15" s="146"/>
+      <c r="D15" s="142" t="s">
+        <v>214</v>
+      </c>
+      <c r="E15" s="141"/>
       <c r="F15" s="54" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G15" s="54"/>
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="144" t="s">
-        <v>216</v>
-      </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="164"/>
-      <c r="E16" s="165"/>
+      <c r="A16" s="146" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="146"/>
+      <c r="C16" s="146"/>
+      <c r="D16" s="142"/>
+      <c r="E16" s="141"/>
       <c r="F16" s="54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G16" s="54"/>
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="144" t="s">
-        <v>214</v>
-      </c>
-      <c r="B17" s="144"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="164"/>
-      <c r="E17" s="165"/>
+      <c r="A17" s="146" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="146"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="142"/>
+      <c r="E17" s="141"/>
       <c r="F17" s="54" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G17" s="54"/>
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="161" t="s">
+      <c r="A18" s="183" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="162"/>
-      <c r="C18" s="163"/>
+      <c r="B18" s="184"/>
+      <c r="C18" s="185"/>
       <c r="D18" s="114"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="145" t="s">
-        <v>179</v>
-      </c>
-      <c r="B19" s="146"/>
-      <c r="C19" s="147"/>
+      <c r="A19" s="169" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="170"/>
+      <c r="C19" s="171"/>
       <c r="D19" s="100"/>
       <c r="E19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -4648,27 +4649,27 @@
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="158" t="s">
-        <v>188</v>
-      </c>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="160"/>
+      <c r="A21" s="180" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="181"/>
+      <c r="C21" s="181"/>
+      <c r="D21" s="181"/>
+      <c r="E21" s="181"/>
+      <c r="F21" s="181"/>
+      <c r="G21" s="182"/>
       <c r="H21" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="101" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B22" s="110"/>
       <c r="C22" s="102"/>
       <c r="D22" s="103" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E22" s="103"/>
       <c r="F22" s="103"/>
@@ -4686,7 +4687,7 @@
       <c r="B23" s="113"/>
       <c r="C23" s="99"/>
       <c r="D23" s="96" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E23" s="97"/>
       <c r="F23" s="97"/>
@@ -4694,7 +4695,7 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="98" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B24" s="113"/>
       <c r="C24" s="99"/>
@@ -4707,28 +4708,28 @@
       <c r="C25"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="157" t="s">
-        <v>189</v>
-      </c>
-      <c r="B26" s="157"/>
-      <c r="C26" s="157"/>
-      <c r="D26" s="157"/>
-      <c r="E26" s="157"/>
-      <c r="F26" s="157"/>
-      <c r="G26" s="157"/>
+      <c r="A26" s="179" t="s">
+        <v>188</v>
+      </c>
+      <c r="B26" s="179"/>
+      <c r="C26" s="179"/>
+      <c r="D26" s="179"/>
+      <c r="E26" s="179"/>
+      <c r="F26" s="179"/>
+      <c r="G26" s="179"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="151" t="s">
-        <v>183</v>
-      </c>
-      <c r="C27" s="152"/>
-      <c r="D27" s="152"/>
-      <c r="E27" s="152"/>
-      <c r="F27" s="152"/>
-      <c r="G27" s="153"/>
+      <c r="B27" s="173" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="174"/>
+      <c r="D27" s="174"/>
+      <c r="E27" s="174"/>
+      <c r="F27" s="174"/>
+      <c r="G27" s="175"/>
       <c r="H27" s="105"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -4739,12 +4740,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="116"/>
-      <c r="B28" s="168"/>
-      <c r="C28" s="168"/>
-      <c r="D28" s="168"/>
-      <c r="E28" s="168"/>
-      <c r="F28" s="168"/>
-      <c r="G28" s="168"/>
+      <c r="B28" s="157"/>
+      <c r="C28" s="157"/>
+      <c r="D28" s="157"/>
+      <c r="E28" s="157"/>
+      <c r="F28" s="157"/>
+      <c r="G28" s="157"/>
       <c r="H28" s="112"/>
       <c r="I28" s="112"/>
       <c r="J28" s="112"/>
@@ -4755,12 +4756,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="117"/>
-      <c r="B29" s="169"/>
-      <c r="C29" s="169"/>
-      <c r="D29" s="169"/>
-      <c r="E29" s="169"/>
-      <c r="F29" s="169"/>
-      <c r="G29" s="169"/>
+      <c r="B29" s="159"/>
+      <c r="C29" s="159"/>
+      <c r="D29" s="159"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="159"/>
+      <c r="G29" s="159"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -4771,12 +4772,12 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="118"/>
-      <c r="B30" s="170"/>
-      <c r="C30" s="170"/>
-      <c r="D30" s="170"/>
-      <c r="E30" s="170"/>
-      <c r="F30" s="170"/>
-      <c r="G30" s="170"/>
+      <c r="B30" s="161"/>
+      <c r="C30" s="161"/>
+      <c r="D30" s="161"/>
+      <c r="E30" s="161"/>
+      <c r="F30" s="161"/>
+      <c r="G30" s="161"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4789,28 +4790,28 @@
       <c r="C31"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="154" t="s">
-        <v>190</v>
-      </c>
-      <c r="B32" s="155"/>
-      <c r="C32" s="155"/>
-      <c r="D32" s="155"/>
-      <c r="E32" s="155"/>
-      <c r="F32" s="155"/>
-      <c r="G32" s="156"/>
+      <c r="A32" s="176" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32" s="177"/>
+      <c r="C32" s="177"/>
+      <c r="D32" s="177"/>
+      <c r="E32" s="177"/>
+      <c r="F32" s="177"/>
+      <c r="G32" s="178"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="174" t="s">
-        <v>184</v>
-      </c>
-      <c r="C33" s="174"/>
-      <c r="D33" s="174"/>
-      <c r="E33" s="174"/>
-      <c r="F33" s="174"/>
-      <c r="G33" s="174"/>
+      <c r="B33" s="153" t="s">
+        <v>183</v>
+      </c>
+      <c r="C33" s="153"/>
+      <c r="D33" s="153"/>
+      <c r="E33" s="153"/>
+      <c r="F33" s="153"/>
+      <c r="G33" s="153"/>
       <c r="H33" s="105"/>
       <c r="I33" s="105"/>
       <c r="J33" s="105"/>
@@ -4823,14 +4824,14 @@
       <c r="A34" s="116">
         <v>1</v>
       </c>
-      <c r="B34" s="175" t="s">
-        <v>218</v>
-      </c>
-      <c r="C34" s="175"/>
-      <c r="D34" s="175"/>
-      <c r="E34" s="175"/>
-      <c r="F34" s="175"/>
-      <c r="G34" s="175"/>
+      <c r="B34" s="154" t="s">
+        <v>217</v>
+      </c>
+      <c r="C34" s="154"/>
+      <c r="D34" s="154"/>
+      <c r="E34" s="154"/>
+      <c r="F34" s="154"/>
+      <c r="G34" s="154"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -4841,12 +4842,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="117"/>
-      <c r="B35" s="176"/>
-      <c r="C35" s="176"/>
-      <c r="D35" s="176"/>
-      <c r="E35" s="176"/>
-      <c r="F35" s="176"/>
-      <c r="G35" s="176"/>
+      <c r="B35" s="155"/>
+      <c r="C35" s="155"/>
+      <c r="D35" s="155"/>
+      <c r="E35" s="155"/>
+      <c r="F35" s="155"/>
+      <c r="G35" s="155"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -4857,12 +4858,12 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="118"/>
-      <c r="B36" s="177"/>
-      <c r="C36" s="177"/>
-      <c r="D36" s="177"/>
-      <c r="E36" s="177"/>
-      <c r="F36" s="177"/>
-      <c r="G36" s="177"/>
+      <c r="B36" s="156"/>
+      <c r="C36" s="156"/>
+      <c r="D36" s="156"/>
+      <c r="E36" s="156"/>
+      <c r="F36" s="156"/>
+      <c r="G36" s="156"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4887,28 +4888,28 @@
       <c r="M37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="154" t="s">
-        <v>191</v>
-      </c>
-      <c r="B38" s="155"/>
-      <c r="C38" s="155"/>
-      <c r="D38" s="155"/>
-      <c r="E38" s="155"/>
-      <c r="F38" s="155"/>
-      <c r="G38" s="156"/>
+      <c r="A38" s="176" t="s">
+        <v>190</v>
+      </c>
+      <c r="B38" s="177"/>
+      <c r="C38" s="177"/>
+      <c r="D38" s="177"/>
+      <c r="E38" s="177"/>
+      <c r="F38" s="177"/>
+      <c r="G38" s="178"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="174" t="s">
-        <v>186</v>
-      </c>
-      <c r="C39" s="174"/>
-      <c r="D39" s="174"/>
-      <c r="E39" s="174"/>
-      <c r="F39" s="174"/>
-      <c r="G39" s="174"/>
+      <c r="B39" s="153" t="s">
+        <v>185</v>
+      </c>
+      <c r="C39" s="153"/>
+      <c r="D39" s="153"/>
+      <c r="E39" s="153"/>
+      <c r="F39" s="153"/>
+      <c r="G39" s="153"/>
       <c r="H39" s="105"/>
       <c r="I39" s="105"/>
       <c r="J39" s="105"/>
@@ -4919,12 +4920,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="116"/>
-      <c r="B40" s="168"/>
-      <c r="C40" s="168"/>
-      <c r="D40" s="168"/>
-      <c r="E40" s="168"/>
-      <c r="F40" s="168"/>
-      <c r="G40" s="178"/>
+      <c r="B40" s="157"/>
+      <c r="C40" s="157"/>
+      <c r="D40" s="157"/>
+      <c r="E40" s="157"/>
+      <c r="F40" s="157"/>
+      <c r="G40" s="158"/>
       <c r="H40" s="112"/>
       <c r="I40" s="112"/>
       <c r="J40" s="112"/>
@@ -4935,12 +4936,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="117"/>
-      <c r="B41" s="169"/>
-      <c r="C41" s="169"/>
-      <c r="D41" s="169"/>
-      <c r="E41" s="169"/>
-      <c r="F41" s="169"/>
-      <c r="G41" s="179"/>
+      <c r="B41" s="159"/>
+      <c r="C41" s="159"/>
+      <c r="D41" s="159"/>
+      <c r="E41" s="159"/>
+      <c r="F41" s="159"/>
+      <c r="G41" s="160"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -4951,12 +4952,12 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="118"/>
-      <c r="B42" s="170"/>
-      <c r="C42" s="170"/>
-      <c r="D42" s="170"/>
-      <c r="E42" s="170"/>
-      <c r="F42" s="170"/>
-      <c r="G42" s="180"/>
+      <c r="B42" s="161"/>
+      <c r="C42" s="161"/>
+      <c r="D42" s="161"/>
+      <c r="E42" s="161"/>
+      <c r="F42" s="161"/>
+      <c r="G42" s="162"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -4991,226 +4992,295 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="141" t="s">
+      <c r="A45" s="166" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="148"/>
-      <c r="C45" s="141" t="s">
+      <c r="B45" s="172"/>
+      <c r="C45" s="166" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="142"/>
-      <c r="E45" s="143"/>
+      <c r="D45" s="167"/>
+      <c r="E45" s="168"/>
       <c r="F45" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="149"/>
-      <c r="B46" s="150"/>
-      <c r="C46" s="149"/>
-      <c r="D46" s="171"/>
-      <c r="E46" s="150"/>
+      <c r="A46" s="163"/>
+      <c r="B46" s="165"/>
+      <c r="C46" s="163"/>
+      <c r="D46" s="164"/>
+      <c r="E46" s="165"/>
       <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="139"/>
-      <c r="B47" s="140"/>
-      <c r="C47" s="139"/>
-      <c r="D47" s="172"/>
-      <c r="E47" s="140"/>
+      <c r="A47" s="147"/>
+      <c r="B47" s="149"/>
+      <c r="C47" s="147"/>
+      <c r="D47" s="148"/>
+      <c r="E47" s="149"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="139"/>
-      <c r="B48" s="140"/>
-      <c r="C48" s="139"/>
-      <c r="D48" s="172"/>
-      <c r="E48" s="140"/>
+      <c r="A48" s="147"/>
+      <c r="B48" s="149"/>
+      <c r="C48" s="147"/>
+      <c r="D48" s="148"/>
+      <c r="E48" s="149"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="139"/>
-      <c r="B49" s="140"/>
-      <c r="C49" s="139"/>
-      <c r="D49" s="172"/>
-      <c r="E49" s="140"/>
+      <c r="A49" s="147"/>
+      <c r="B49" s="149"/>
+      <c r="C49" s="147"/>
+      <c r="D49" s="148"/>
+      <c r="E49" s="149"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="139"/>
-      <c r="B50" s="140"/>
-      <c r="C50" s="139"/>
-      <c r="D50" s="172"/>
-      <c r="E50" s="140"/>
+      <c r="A50" s="147"/>
+      <c r="B50" s="149"/>
+      <c r="C50" s="147"/>
+      <c r="D50" s="148"/>
+      <c r="E50" s="149"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="139"/>
-      <c r="B51" s="140"/>
-      <c r="C51" s="139"/>
-      <c r="D51" s="172"/>
-      <c r="E51" s="140"/>
+      <c r="A51" s="147"/>
+      <c r="B51" s="149"/>
+      <c r="C51" s="147"/>
+      <c r="D51" s="148"/>
+      <c r="E51" s="149"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="139"/>
-      <c r="B52" s="140"/>
-      <c r="C52" s="139"/>
-      <c r="D52" s="172"/>
-      <c r="E52" s="140"/>
+      <c r="A52" s="147"/>
+      <c r="B52" s="149"/>
+      <c r="C52" s="147"/>
+      <c r="D52" s="148"/>
+      <c r="E52" s="149"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="139"/>
-      <c r="B53" s="140"/>
-      <c r="C53" s="139"/>
-      <c r="D53" s="172"/>
-      <c r="E53" s="140"/>
+      <c r="A53" s="147"/>
+      <c r="B53" s="149"/>
+      <c r="C53" s="147"/>
+      <c r="D53" s="148"/>
+      <c r="E53" s="149"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="139"/>
-      <c r="B54" s="140"/>
-      <c r="C54" s="139"/>
-      <c r="D54" s="172"/>
-      <c r="E54" s="140"/>
+      <c r="A54" s="147"/>
+      <c r="B54" s="149"/>
+      <c r="C54" s="147"/>
+      <c r="D54" s="148"/>
+      <c r="E54" s="149"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="139"/>
-      <c r="B55" s="140"/>
-      <c r="C55" s="139"/>
-      <c r="D55" s="172"/>
-      <c r="E55" s="140"/>
+      <c r="A55" s="147"/>
+      <c r="B55" s="149"/>
+      <c r="C55" s="147"/>
+      <c r="D55" s="148"/>
+      <c r="E55" s="149"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="139"/>
-      <c r="B56" s="140"/>
-      <c r="C56" s="139"/>
-      <c r="D56" s="172"/>
-      <c r="E56" s="140"/>
+      <c r="A56" s="147"/>
+      <c r="B56" s="149"/>
+      <c r="C56" s="147"/>
+      <c r="D56" s="148"/>
+      <c r="E56" s="149"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="139"/>
-      <c r="B57" s="140"/>
-      <c r="C57" s="139"/>
-      <c r="D57" s="172"/>
-      <c r="E57" s="140"/>
+      <c r="A57" s="147"/>
+      <c r="B57" s="149"/>
+      <c r="C57" s="147"/>
+      <c r="D57" s="148"/>
+      <c r="E57" s="149"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="139"/>
-      <c r="B58" s="140"/>
-      <c r="C58" s="139"/>
-      <c r="D58" s="172"/>
-      <c r="E58" s="140"/>
+      <c r="A58" s="147"/>
+      <c r="B58" s="149"/>
+      <c r="C58" s="147"/>
+      <c r="D58" s="148"/>
+      <c r="E58" s="149"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="139"/>
-      <c r="B59" s="140"/>
-      <c r="C59" s="139"/>
-      <c r="D59" s="172"/>
-      <c r="E59" s="140"/>
+      <c r="A59" s="147"/>
+      <c r="B59" s="149"/>
+      <c r="C59" s="147"/>
+      <c r="D59" s="148"/>
+      <c r="E59" s="149"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="139"/>
-      <c r="B60" s="140"/>
-      <c r="C60" s="139"/>
-      <c r="D60" s="172"/>
-      <c r="E60" s="140"/>
+      <c r="A60" s="147"/>
+      <c r="B60" s="149"/>
+      <c r="C60" s="147"/>
+      <c r="D60" s="148"/>
+      <c r="E60" s="149"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="139"/>
-      <c r="B61" s="140"/>
-      <c r="C61" s="139"/>
-      <c r="D61" s="172"/>
-      <c r="E61" s="140"/>
+      <c r="A61" s="147"/>
+      <c r="B61" s="149"/>
+      <c r="C61" s="147"/>
+      <c r="D61" s="148"/>
+      <c r="E61" s="149"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="139"/>
-      <c r="B62" s="140"/>
-      <c r="C62" s="139"/>
-      <c r="D62" s="172"/>
-      <c r="E62" s="140"/>
+      <c r="A62" s="147"/>
+      <c r="B62" s="149"/>
+      <c r="C62" s="147"/>
+      <c r="D62" s="148"/>
+      <c r="E62" s="149"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="139"/>
-      <c r="B63" s="140"/>
-      <c r="C63" s="139"/>
-      <c r="D63" s="172"/>
-      <c r="E63" s="140"/>
+      <c r="A63" s="147"/>
+      <c r="B63" s="149"/>
+      <c r="C63" s="147"/>
+      <c r="D63" s="148"/>
+      <c r="E63" s="149"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="139"/>
-      <c r="B64" s="140"/>
-      <c r="C64" s="139"/>
-      <c r="D64" s="172"/>
-      <c r="E64" s="140"/>
+      <c r="A64" s="147"/>
+      <c r="B64" s="149"/>
+      <c r="C64" s="147"/>
+      <c r="D64" s="148"/>
+      <c r="E64" s="149"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="139"/>
-      <c r="B65" s="140"/>
-      <c r="C65" s="139"/>
-      <c r="D65" s="172"/>
-      <c r="E65" s="140"/>
+      <c r="A65" s="147"/>
+      <c r="B65" s="149"/>
+      <c r="C65" s="147"/>
+      <c r="D65" s="148"/>
+      <c r="E65" s="149"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="139"/>
-      <c r="B66" s="140"/>
-      <c r="C66" s="139"/>
-      <c r="D66" s="172"/>
-      <c r="E66" s="140"/>
+      <c r="A66" s="147"/>
+      <c r="B66" s="149"/>
+      <c r="C66" s="147"/>
+      <c r="D66" s="148"/>
+      <c r="E66" s="149"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="139"/>
-      <c r="B67" s="140"/>
-      <c r="C67" s="139"/>
-      <c r="D67" s="172"/>
-      <c r="E67" s="140"/>
+      <c r="A67" s="147"/>
+      <c r="B67" s="149"/>
+      <c r="C67" s="147"/>
+      <c r="D67" s="148"/>
+      <c r="E67" s="149"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="139"/>
-      <c r="B68" s="140"/>
-      <c r="C68" s="139"/>
-      <c r="D68" s="172"/>
-      <c r="E68" s="140"/>
+      <c r="A68" s="147"/>
+      <c r="B68" s="149"/>
+      <c r="C68" s="147"/>
+      <c r="D68" s="148"/>
+      <c r="E68" s="149"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="139"/>
-      <c r="B69" s="140"/>
-      <c r="C69" s="139"/>
-      <c r="D69" s="172"/>
-      <c r="E69" s="140"/>
+      <c r="A69" s="147"/>
+      <c r="B69" s="149"/>
+      <c r="C69" s="147"/>
+      <c r="D69" s="148"/>
+      <c r="E69" s="149"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="166"/>
-      <c r="B70" s="167"/>
-      <c r="C70" s="166"/>
-      <c r="D70" s="173"/>
-      <c r="E70" s="167"/>
+      <c r="A70" s="150"/>
+      <c r="B70" s="152"/>
+      <c r="C70" s="150"/>
+      <c r="D70" s="151"/>
+      <c r="E70" s="152"/>
       <c r="F70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C59:E59"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
@@ -5227,80 +5297,11 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -5431,7 +5432,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D7" s="127"/>
       <c r="E7" s="54"/>
@@ -5460,7 +5461,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
       <c r="I8" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
@@ -5542,7 +5543,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D14" s="35"/>
       <c r="E14" s="54"/>
@@ -5555,15 +5556,15 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="122" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="122"/>
+      <c r="C15" s="141" t="s">
         <v>174</v>
       </c>
-      <c r="B15" s="122"/>
-      <c r="C15" s="165" t="s">
+      <c r="D15" s="141"/>
+      <c r="E15" s="95" t="s">
         <v>175</v>
-      </c>
-      <c r="D15" s="165"/>
-      <c r="E15" s="95" t="s">
-        <v>176</v>
       </c>
       <c r="G15" s="54"/>
       <c r="I15"/>
@@ -5573,15 +5574,15 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="122" t="s">
+        <v>225</v>
+      </c>
+      <c r="B16" s="122"/>
+      <c r="C16" s="142" t="s">
+        <v>229</v>
+      </c>
+      <c r="D16" s="141"/>
+      <c r="E16" s="55" t="s">
         <v>226</v>
-      </c>
-      <c r="B16" s="122"/>
-      <c r="C16" s="164" t="s">
-        <v>230</v>
-      </c>
-      <c r="D16" s="165"/>
-      <c r="E16" s="55" t="s">
-        <v>227</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
@@ -5596,13 +5597,13 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="122" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="122"/>
+      <c r="C17" s="141" t="s">
         <v>177</v>
       </c>
-      <c r="B17" s="122"/>
-      <c r="C17" s="165" t="s">
-        <v>178</v>
-      </c>
-      <c r="D17" s="165"/>
+      <c r="D17" s="141"/>
       <c r="E17" s="55"/>
       <c r="F17" s="55"/>
       <c r="G17" s="54"/>
@@ -5611,13 +5612,13 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="122" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18" s="122"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="55" t="s">
         <v>228</v>
-      </c>
-      <c r="B18" s="122"/>
-      <c r="C18" s="164"/>
-      <c r="D18" s="165"/>
-      <c r="E18" s="55" t="s">
-        <v>229</v>
       </c>
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
@@ -5632,14 +5633,14 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="123" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B19" s="124"/>
       <c r="C19" s="100" t="s">
         <v>141</v>
       </c>
       <c r="D19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
@@ -5665,15 +5666,15 @@
       <c r="L20"/>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" s="157" t="s">
-        <v>192</v>
-      </c>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
+      <c r="A21" s="179" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="179"/>
+      <c r="C21" s="179"/>
+      <c r="D21" s="179"/>
+      <c r="E21" s="179"/>
+      <c r="F21" s="179"/>
+      <c r="G21" s="179"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -5683,14 +5684,14 @@
       <c r="A22" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="151" t="s">
-        <v>183</v>
-      </c>
-      <c r="C22" s="152"/>
-      <c r="D22" s="152"/>
-      <c r="E22" s="152"/>
-      <c r="F22" s="152"/>
-      <c r="G22" s="153"/>
+      <c r="B22" s="173" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="174"/>
+      <c r="D22" s="174"/>
+      <c r="E22" s="174"/>
+      <c r="F22" s="174"/>
+      <c r="G22" s="175"/>
       <c r="H22" s="105"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -5708,12 +5709,12 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="116"/>
-      <c r="B23" s="168"/>
-      <c r="C23" s="168"/>
-      <c r="D23" s="168"/>
-      <c r="E23" s="168"/>
-      <c r="F23" s="168"/>
-      <c r="G23" s="168"/>
+      <c r="B23" s="157"/>
+      <c r="C23" s="157"/>
+      <c r="D23" s="157"/>
+      <c r="E23" s="157"/>
+      <c r="F23" s="157"/>
+      <c r="G23" s="157"/>
       <c r="H23" s="112"/>
       <c r="I23"/>
       <c r="J23"/>
@@ -5731,12 +5732,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="117"/>
-      <c r="B24" s="169"/>
-      <c r="C24" s="169"/>
-      <c r="D24" s="169"/>
-      <c r="E24" s="169"/>
-      <c r="F24" s="169"/>
-      <c r="G24" s="169"/>
+      <c r="B24" s="159"/>
+      <c r="C24" s="159"/>
+      <c r="D24" s="159"/>
+      <c r="E24" s="159"/>
+      <c r="F24" s="159"/>
+      <c r="G24" s="159"/>
       <c r="H24" s="112"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -5754,12 +5755,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="118"/>
-      <c r="B25" s="170"/>
-      <c r="C25" s="170"/>
-      <c r="D25" s="170"/>
-      <c r="E25" s="170"/>
-      <c r="F25" s="170"/>
-      <c r="G25" s="170"/>
+      <c r="B25" s="161"/>
+      <c r="C25" s="161"/>
+      <c r="D25" s="161"/>
+      <c r="E25" s="161"/>
+      <c r="F25" s="161"/>
+      <c r="G25" s="161"/>
       <c r="H25" s="112"/>
       <c r="M25" s="112"/>
       <c r="N25" s="112"/>
@@ -5779,15 +5780,15 @@
       <c r="L26" s="105"/>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="154" t="s">
-        <v>193</v>
-      </c>
-      <c r="B27" s="155"/>
-      <c r="C27" s="155"/>
-      <c r="D27" s="155"/>
-      <c r="E27" s="155"/>
-      <c r="F27" s="155"/>
-      <c r="G27" s="156"/>
+      <c r="A27" s="176" t="s">
+        <v>192</v>
+      </c>
+      <c r="B27" s="177"/>
+      <c r="C27" s="177"/>
+      <c r="D27" s="177"/>
+      <c r="E27" s="177"/>
+      <c r="F27" s="177"/>
+      <c r="G27" s="178"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
       <c r="K27" s="105"/>
@@ -5797,14 +5798,14 @@
       <c r="A28" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="174" t="s">
-        <v>184</v>
-      </c>
-      <c r="C28" s="174"/>
-      <c r="D28" s="174"/>
-      <c r="E28" s="174"/>
-      <c r="F28" s="174"/>
-      <c r="G28" s="174"/>
+      <c r="B28" s="153" t="s">
+        <v>183</v>
+      </c>
+      <c r="C28" s="153"/>
+      <c r="D28" s="153"/>
+      <c r="E28" s="153"/>
+      <c r="F28" s="153"/>
+      <c r="G28" s="153"/>
       <c r="H28" s="105"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -5824,14 +5825,14 @@
       <c r="A29" s="116">
         <v>1</v>
       </c>
-      <c r="B29" s="175" t="s">
-        <v>225</v>
-      </c>
-      <c r="C29" s="175"/>
-      <c r="D29" s="175"/>
-      <c r="E29" s="175"/>
-      <c r="F29" s="175"/>
-      <c r="G29" s="175"/>
+      <c r="B29" s="154" t="s">
+        <v>224</v>
+      </c>
+      <c r="C29" s="154"/>
+      <c r="D29" s="154"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="154"/>
       <c r="H29" s="112"/>
       <c r="I29"/>
       <c r="J29"/>
@@ -5849,12 +5850,12 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="117"/>
-      <c r="B30" s="176"/>
-      <c r="C30" s="176"/>
-      <c r="D30" s="176"/>
-      <c r="E30" s="176"/>
-      <c r="F30" s="176"/>
-      <c r="G30" s="176"/>
+      <c r="B30" s="155"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="155"/>
+      <c r="G30" s="155"/>
       <c r="H30" s="112"/>
       <c r="M30" s="112"/>
       <c r="N30" s="112"/>
@@ -5868,12 +5869,12 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="118"/>
-      <c r="B31" s="177"/>
-      <c r="C31" s="177"/>
-      <c r="D31" s="177"/>
-      <c r="E31" s="177"/>
-      <c r="F31" s="177"/>
-      <c r="G31" s="177"/>
+      <c r="B31" s="156"/>
+      <c r="C31" s="156"/>
+      <c r="D31" s="156"/>
+      <c r="E31" s="156"/>
+      <c r="F31" s="156"/>
+      <c r="G31" s="156"/>
       <c r="H31" s="112"/>
       <c r="I31" s="105"/>
       <c r="J31" s="105"/>
@@ -5912,15 +5913,15 @@
       <c r="T32"/>
     </row>
     <row r="33" spans="1:26">
-      <c r="A33" s="154" t="s">
-        <v>194</v>
-      </c>
-      <c r="B33" s="155"/>
-      <c r="C33" s="155"/>
-      <c r="D33" s="155"/>
-      <c r="E33" s="155"/>
-      <c r="F33" s="155"/>
-      <c r="G33" s="156"/>
+      <c r="A33" s="176" t="s">
+        <v>193</v>
+      </c>
+      <c r="B33" s="177"/>
+      <c r="C33" s="177"/>
+      <c r="D33" s="177"/>
+      <c r="E33" s="177"/>
+      <c r="F33" s="177"/>
+      <c r="G33" s="178"/>
       <c r="I33" s="112"/>
       <c r="J33" s="112"/>
       <c r="K33" s="112"/>
@@ -5930,14 +5931,14 @@
       <c r="A34" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="174" t="s">
-        <v>186</v>
-      </c>
-      <c r="C34" s="174"/>
-      <c r="D34" s="174"/>
-      <c r="E34" s="174"/>
-      <c r="F34" s="174"/>
-      <c r="G34" s="174"/>
+      <c r="B34" s="153" t="s">
+        <v>185</v>
+      </c>
+      <c r="C34" s="153"/>
+      <c r="D34" s="153"/>
+      <c r="E34" s="153"/>
+      <c r="F34" s="153"/>
+      <c r="G34" s="153"/>
       <c r="H34" s="105"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -5955,12 +5956,12 @@
     </row>
     <row r="35" spans="1:26">
       <c r="A35" s="116"/>
-      <c r="B35" s="168"/>
-      <c r="C35" s="168"/>
-      <c r="D35" s="168"/>
-      <c r="E35" s="168"/>
-      <c r="F35" s="168"/>
-      <c r="G35" s="178"/>
+      <c r="B35" s="157"/>
+      <c r="C35" s="157"/>
+      <c r="D35" s="157"/>
+      <c r="E35" s="157"/>
+      <c r="F35" s="157"/>
+      <c r="G35" s="158"/>
       <c r="H35" s="112"/>
       <c r="I35"/>
       <c r="J35"/>
@@ -5978,12 +5979,12 @@
     </row>
     <row r="36" spans="1:26">
       <c r="A36" s="117"/>
-      <c r="B36" s="169"/>
-      <c r="C36" s="169"/>
-      <c r="D36" s="169"/>
-      <c r="E36" s="169"/>
-      <c r="F36" s="169"/>
-      <c r="G36" s="179"/>
+      <c r="B36" s="159"/>
+      <c r="C36" s="159"/>
+      <c r="D36" s="159"/>
+      <c r="E36" s="159"/>
+      <c r="F36" s="159"/>
+      <c r="G36" s="160"/>
       <c r="H36" s="112"/>
       <c r="M36" s="112"/>
       <c r="N36" s="112"/>
@@ -5997,12 +5998,12 @@
     </row>
     <row r="37" spans="1:26">
       <c r="A37" s="118"/>
-      <c r="B37" s="170"/>
-      <c r="C37" s="170"/>
-      <c r="D37" s="170"/>
-      <c r="E37" s="170"/>
-      <c r="F37" s="170"/>
-      <c r="G37" s="180"/>
+      <c r="B37" s="161"/>
+      <c r="C37" s="161"/>
+      <c r="D37" s="161"/>
+      <c r="E37" s="161"/>
+      <c r="F37" s="161"/>
+      <c r="G37" s="162"/>
       <c r="H37" s="112"/>
       <c r="M37" s="112"/>
       <c r="N37" s="112"/>
@@ -6066,82 +6067,82 @@
       <c r="Z40" s="39"/>
     </row>
     <row r="41" spans="1:26">
-      <c r="A41" s="190" t="s">
+      <c r="A41" s="186" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="190" t="s">
+      <c r="B41" s="186" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="192" t="s">
+      <c r="C41" s="188" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="190" t="s">
+      <c r="D41" s="186" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="193" t="s">
+      <c r="E41" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="F41" s="193" t="s">
-        <v>177</v>
-      </c>
-      <c r="G41" s="190" t="s">
+      <c r="F41" s="189" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="190" t="s">
+      <c r="H41" s="186" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="197" t="s">
+      <c r="I41" s="193" t="s">
+        <v>199</v>
+      </c>
+      <c r="J41" s="193" t="s">
         <v>200</v>
       </c>
-      <c r="J41" s="197" t="s">
+      <c r="K41" s="193" t="s">
         <v>201</v>
       </c>
-      <c r="K41" s="197" t="s">
+      <c r="L41" s="196" t="s">
         <v>202</v>
       </c>
-      <c r="L41" s="186" t="s">
-        <v>203</v>
-      </c>
-      <c r="M41" s="190" t="s">
-        <v>195</v>
-      </c>
-      <c r="N41" s="190" t="s">
-        <v>209</v>
-      </c>
-      <c r="O41" s="192" t="s">
+      <c r="M41" s="186" t="s">
+        <v>194</v>
+      </c>
+      <c r="N41" s="186" t="s">
         <v>208</v>
       </c>
-      <c r="P41" s="188" t="s">
+      <c r="O41" s="188" t="s">
+        <v>207</v>
+      </c>
+      <c r="P41" s="194" t="s">
         <v>71</v>
       </c>
-      <c r="Q41" s="189"/>
-      <c r="R41" s="188" t="s">
+      <c r="Q41" s="195"/>
+      <c r="R41" s="194" t="s">
         <v>17</v>
       </c>
-      <c r="S41" s="189"/>
+      <c r="S41" s="195"/>
       <c r="T41" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="U41" s="190" t="s">
+      <c r="U41" s="186" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:26">
-      <c r="A42" s="191"/>
-      <c r="B42" s="191"/>
-      <c r="C42" s="191"/>
-      <c r="D42" s="191"/>
-      <c r="E42" s="194"/>
-      <c r="F42" s="195"/>
-      <c r="G42" s="191"/>
-      <c r="H42" s="191"/>
-      <c r="I42" s="197"/>
-      <c r="J42" s="197"/>
-      <c r="K42" s="197"/>
-      <c r="L42" s="187"/>
-      <c r="M42" s="196"/>
-      <c r="N42" s="196"/>
-      <c r="O42" s="196"/>
+      <c r="A42" s="187"/>
+      <c r="B42" s="187"/>
+      <c r="C42" s="187"/>
+      <c r="D42" s="187"/>
+      <c r="E42" s="190"/>
+      <c r="F42" s="191"/>
+      <c r="G42" s="187"/>
+      <c r="H42" s="187"/>
+      <c r="I42" s="193"/>
+      <c r="J42" s="193"/>
+      <c r="K42" s="193"/>
+      <c r="L42" s="197"/>
+      <c r="M42" s="192"/>
+      <c r="N42" s="192"/>
+      <c r="O42" s="192"/>
       <c r="P42" s="29" t="s">
         <v>75</v>
       </c>
@@ -6157,7 +6158,7 @@
       <c r="T42" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U42" s="191"/>
+      <c r="U42" s="187"/>
     </row>
     <row r="43" spans="1:26" ht="30">
       <c r="A43" s="7">
@@ -6179,11 +6180,11 @@
       </c>
       <c r="H43" s="24"/>
       <c r="I43" s="133" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J43" s="133"/>
       <c r="K43" s="138" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L43" s="133"/>
       <c r="M43" s="24" t="s">
@@ -6227,11 +6228,11 @@
       </c>
       <c r="H44" s="25"/>
       <c r="I44" s="135" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J44" s="135"/>
       <c r="K44" s="136" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L44" s="135"/>
       <c r="M44" s="25" t="s">
@@ -6343,7 +6344,7 @@
         <v>111</v>
       </c>
       <c r="E47" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F47" s="26"/>
       <c r="G47" s="86"/>
@@ -6367,7 +6368,7 @@
       <c r="S47" s="32"/>
       <c r="T47" s="32"/>
       <c r="U47" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:26">
@@ -6416,7 +6417,7 @@
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="26"/>
@@ -6835,6 +6836,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B35:G35"/>
     <mergeCell ref="U41:U42"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="B41:B42"/>
@@ -6851,27 +6873,6 @@
     <mergeCell ref="M41:M42"/>
     <mergeCell ref="R41:S41"/>
     <mergeCell ref="N41:N42"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="P41:Q41"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="L41:L42"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -6928,7 +6929,7 @@
   </sheetPr>
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -7021,7 +7022,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="54"/>
@@ -7048,7 +7049,7 @@
       <c r="F8" s="54"/>
       <c r="H8" s="28"/>
       <c r="I8" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
@@ -7090,7 +7091,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="54"/>
@@ -7101,15 +7102,15 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="122" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="122"/>
+      <c r="C12" s="141" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="122"/>
-      <c r="C12" s="165" t="s">
+      <c r="D12" s="141"/>
+      <c r="E12" s="95" t="s">
         <v>175</v>
-      </c>
-      <c r="D12" s="165"/>
-      <c r="E12" s="95" t="s">
-        <v>176</v>
       </c>
       <c r="F12" s="95"/>
       <c r="H12" s="54"/>
@@ -7119,15 +7120,15 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="122" t="s">
+        <v>225</v>
+      </c>
+      <c r="B13" s="122"/>
+      <c r="C13" s="142" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="141"/>
+      <c r="E13" s="55" t="s">
         <v>226</v>
-      </c>
-      <c r="B13" s="122"/>
-      <c r="C13" s="164" t="s">
-        <v>230</v>
-      </c>
-      <c r="D13" s="165"/>
-      <c r="E13" s="55" t="s">
-        <v>227</v>
       </c>
       <c r="F13" s="54"/>
       <c r="G13" s="54"/>
@@ -7142,13 +7143,13 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="122" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="122"/>
+      <c r="C14" s="141" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="122"/>
-      <c r="C14" s="165" t="s">
-        <v>178</v>
-      </c>
-      <c r="D14" s="165"/>
+      <c r="D14" s="141"/>
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="54"/>
@@ -7157,13 +7158,13 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="122" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" s="122"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="141"/>
+      <c r="E15" s="55" t="s">
         <v>228</v>
-      </c>
-      <c r="B15" s="122"/>
-      <c r="C15" s="164"/>
-      <c r="D15" s="165"/>
-      <c r="E15" s="55" t="s">
-        <v>229</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
@@ -7178,14 +7179,14 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="123" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" s="124"/>
       <c r="C16" s="100" t="s">
         <v>141</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
@@ -7209,15 +7210,15 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="157" t="s">
-        <v>192</v>
-      </c>
-      <c r="B18" s="157"/>
-      <c r="C18" s="157"/>
-      <c r="D18" s="157"/>
-      <c r="E18" s="157"/>
-      <c r="F18" s="157"/>
-      <c r="G18" s="157"/>
+      <c r="A18" s="179" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18" s="179"/>
+      <c r="C18" s="179"/>
+      <c r="D18" s="179"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="179"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -7228,14 +7229,14 @@
       <c r="A19" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="151" t="s">
-        <v>183</v>
-      </c>
-      <c r="C19" s="152"/>
-      <c r="D19" s="152"/>
-      <c r="E19" s="152"/>
-      <c r="F19" s="152"/>
-      <c r="G19" s="153"/>
+      <c r="B19" s="173" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="174"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="174"/>
+      <c r="F19" s="174"/>
+      <c r="G19" s="175"/>
       <c r="H19" s="105"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -7251,12 +7252,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="116"/>
-      <c r="B20" s="168"/>
-      <c r="C20" s="168"/>
-      <c r="D20" s="168"/>
-      <c r="E20" s="168"/>
-      <c r="F20" s="168"/>
-      <c r="G20" s="168"/>
+      <c r="B20" s="157"/>
+      <c r="C20" s="157"/>
+      <c r="D20" s="157"/>
+      <c r="E20" s="157"/>
+      <c r="F20" s="157"/>
+      <c r="G20" s="157"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -7271,12 +7272,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="117"/>
-      <c r="B21" s="169"/>
-      <c r="C21" s="169"/>
-      <c r="D21" s="169"/>
-      <c r="E21" s="169"/>
-      <c r="F21" s="169"/>
-      <c r="G21" s="169"/>
+      <c r="B21" s="159"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="159"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -7291,12 +7292,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="118"/>
-      <c r="B22" s="170"/>
-      <c r="C22" s="170"/>
-      <c r="D22" s="170"/>
-      <c r="E22" s="170"/>
-      <c r="F22" s="170"/>
-      <c r="G22" s="170"/>
+      <c r="B22" s="161"/>
+      <c r="C22" s="161"/>
+      <c r="D22" s="161"/>
+      <c r="E22" s="161"/>
+      <c r="F22" s="161"/>
+      <c r="G22" s="161"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -7323,15 +7324,15 @@
       <c r="O23" s="112"/>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="154" t="s">
-        <v>193</v>
-      </c>
-      <c r="B24" s="155"/>
-      <c r="C24" s="155"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="155"/>
-      <c r="F24" s="155"/>
-      <c r="G24" s="156"/>
+      <c r="A24" s="176" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="177"/>
+      <c r="C24" s="177"/>
+      <c r="D24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="178"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -7344,14 +7345,14 @@
       <c r="A25" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="174" t="s">
-        <v>184</v>
-      </c>
-      <c r="C25" s="174"/>
-      <c r="D25" s="174"/>
-      <c r="E25" s="174"/>
-      <c r="F25" s="174"/>
-      <c r="G25" s="174"/>
+      <c r="B25" s="153" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" s="153"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="153"/>
+      <c r="F25" s="153"/>
+      <c r="G25" s="153"/>
       <c r="H25" s="105"/>
       <c r="M25" s="112"/>
       <c r="N25" s="112"/>
@@ -7367,14 +7368,14 @@
       <c r="A26" s="116">
         <v>1</v>
       </c>
-      <c r="B26" s="175" t="s">
-        <v>185</v>
-      </c>
-      <c r="C26" s="175"/>
-      <c r="D26" s="175"/>
-      <c r="E26" s="175"/>
-      <c r="F26" s="175"/>
-      <c r="G26" s="175"/>
+      <c r="B26" s="154" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="154"/>
+      <c r="D26" s="154"/>
+      <c r="E26" s="154"/>
+      <c r="F26" s="154"/>
+      <c r="G26" s="154"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7389,12 +7390,12 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="117"/>
-      <c r="B27" s="176"/>
-      <c r="C27" s="176"/>
-      <c r="D27" s="176"/>
-      <c r="E27" s="176"/>
-      <c r="F27" s="176"/>
-      <c r="G27" s="176"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="155"/>
+      <c r="D27" s="155"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="155"/>
+      <c r="G27" s="155"/>
       <c r="H27" s="112"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -7409,12 +7410,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="118"/>
-      <c r="B28" s="177"/>
-      <c r="C28" s="177"/>
-      <c r="D28" s="177"/>
-      <c r="E28" s="177"/>
-      <c r="F28" s="177"/>
-      <c r="G28" s="177"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
       <c r="H28" s="112"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -7453,15 +7454,15 @@
       <c r="T29"/>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="154" t="s">
-        <v>194</v>
-      </c>
-      <c r="B30" s="155"/>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="156"/>
+      <c r="A30" s="176" t="s">
+        <v>193</v>
+      </c>
+      <c r="B30" s="177"/>
+      <c r="C30" s="177"/>
+      <c r="D30" s="177"/>
+      <c r="E30" s="177"/>
+      <c r="F30" s="177"/>
+      <c r="G30" s="178"/>
       <c r="M30" s="112"/>
       <c r="N30" s="112"/>
       <c r="O30" s="112"/>
@@ -7470,14 +7471,14 @@
       <c r="A31" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="174" t="s">
-        <v>186</v>
-      </c>
-      <c r="C31" s="174"/>
-      <c r="D31" s="174"/>
-      <c r="E31" s="174"/>
-      <c r="F31" s="174"/>
-      <c r="G31" s="174"/>
+      <c r="B31" s="153" t="s">
+        <v>185</v>
+      </c>
+      <c r="C31" s="153"/>
+      <c r="D31" s="153"/>
+      <c r="E31" s="153"/>
+      <c r="F31" s="153"/>
+      <c r="G31" s="153"/>
       <c r="H31" s="105"/>
       <c r="I31" s="105"/>
       <c r="J31" s="105"/>
@@ -7495,12 +7496,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="116"/>
-      <c r="B32" s="168"/>
-      <c r="C32" s="168"/>
-      <c r="D32" s="168"/>
-      <c r="E32" s="168"/>
-      <c r="F32" s="168"/>
-      <c r="G32" s="178"/>
+      <c r="B32" s="157"/>
+      <c r="C32" s="157"/>
+      <c r="D32" s="157"/>
+      <c r="E32" s="157"/>
+      <c r="F32" s="157"/>
+      <c r="G32" s="158"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7518,12 +7519,12 @@
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="117"/>
-      <c r="B33" s="169"/>
-      <c r="C33" s="169"/>
-      <c r="D33" s="169"/>
-      <c r="E33" s="169"/>
-      <c r="F33" s="169"/>
-      <c r="G33" s="179"/>
+      <c r="B33" s="159"/>
+      <c r="C33" s="159"/>
+      <c r="D33" s="159"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="160"/>
       <c r="H33" s="112"/>
       <c r="I33" s="112"/>
       <c r="J33" s="112"/>
@@ -7538,12 +7539,12 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="118"/>
-      <c r="B34" s="170"/>
-      <c r="C34" s="170"/>
-      <c r="D34" s="170"/>
-      <c r="E34" s="170"/>
-      <c r="F34" s="170"/>
-      <c r="G34" s="180"/>
+      <c r="B34" s="161"/>
+      <c r="C34" s="161"/>
+      <c r="D34" s="161"/>
+      <c r="E34" s="161"/>
+      <c r="F34" s="161"/>
+      <c r="G34" s="162"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -7613,84 +7614,84 @@
       <c r="U37" s="58"/>
     </row>
     <row r="38" spans="1:22" ht="30" customHeight="1">
-      <c r="A38" s="193" t="s">
+      <c r="A38" s="189" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="193" t="s">
+      <c r="B38" s="189" t="s">
         <v>119</v>
       </c>
       <c r="C38" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="193" t="s">
+      <c r="D38" s="189" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="193" t="s">
+      <c r="E38" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="193" t="s">
-        <v>177</v>
-      </c>
-      <c r="G38" s="193" t="s">
+      <c r="F38" s="189" t="s">
+        <v>176</v>
+      </c>
+      <c r="G38" s="189" t="s">
         <v>140</v>
       </c>
-      <c r="H38" s="193" t="s">
+      <c r="H38" s="189" t="s">
         <v>139</v>
       </c>
-      <c r="I38" s="201" t="s">
+      <c r="I38" s="203" t="s">
+        <v>199</v>
+      </c>
+      <c r="J38" s="205" t="s">
         <v>200</v>
       </c>
-      <c r="J38" s="203" t="s">
+      <c r="K38" s="205" t="s">
         <v>201</v>
       </c>
-      <c r="K38" s="203" t="s">
+      <c r="L38" s="196" t="s">
         <v>202</v>
       </c>
-      <c r="L38" s="186" t="s">
-        <v>203</v>
-      </c>
-      <c r="M38" s="190" t="s">
-        <v>195</v>
-      </c>
-      <c r="N38" s="190" t="s">
-        <v>209</v>
-      </c>
-      <c r="O38" s="192" t="s">
+      <c r="M38" s="186" t="s">
+        <v>194</v>
+      </c>
+      <c r="N38" s="186" t="s">
         <v>208</v>
       </c>
-      <c r="P38" s="199" t="s">
+      <c r="O38" s="188" t="s">
+        <v>207</v>
+      </c>
+      <c r="P38" s="202" t="s">
         <v>122</v>
       </c>
       <c r="Q38" s="200"/>
-      <c r="R38" s="206" t="s">
+      <c r="R38" s="199" t="s">
         <v>123</v>
       </c>
       <c r="S38" s="200"/>
       <c r="T38" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U38" s="193" t="s">
+      <c r="U38" s="189" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15">
-      <c r="A39" s="198"/>
-      <c r="B39" s="198"/>
+      <c r="A39" s="201"/>
+      <c r="B39" s="201"/>
       <c r="C39" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="198"/>
-      <c r="E39" s="195"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="198"/>
-      <c r="H39" s="198"/>
-      <c r="I39" s="202"/>
-      <c r="J39" s="204"/>
-      <c r="K39" s="204"/>
-      <c r="L39" s="187"/>
-      <c r="M39" s="196"/>
-      <c r="N39" s="196"/>
-      <c r="O39" s="205"/>
+      <c r="D39" s="201"/>
+      <c r="E39" s="191"/>
+      <c r="F39" s="191"/>
+      <c r="G39" s="201"/>
+      <c r="H39" s="201"/>
+      <c r="I39" s="204"/>
+      <c r="J39" s="206"/>
+      <c r="K39" s="206"/>
+      <c r="L39" s="197"/>
+      <c r="M39" s="192"/>
+      <c r="N39" s="192"/>
+      <c r="O39" s="198"/>
       <c r="P39" s="62" t="s">
         <v>126</v>
       </c>
@@ -7706,7 +7707,7 @@
       <c r="T39" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="U39" s="198"/>
+      <c r="U39" s="201"/>
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="64">
@@ -7728,11 +7729,11 @@
       </c>
       <c r="H40" s="67"/>
       <c r="I40" s="133" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J40" s="133"/>
       <c r="K40" s="134" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L40" s="133"/>
       <c r="M40" s="24" t="s">
@@ -7771,11 +7772,11 @@
       </c>
       <c r="H41" s="67"/>
       <c r="I41" s="135" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J41" s="135"/>
       <c r="K41" s="136" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L41" s="135"/>
       <c r="M41" s="25" t="s">
@@ -7878,7 +7879,7 @@
         <v>110</v>
       </c>
       <c r="E44" s="74" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F44" s="74"/>
       <c r="G44" s="91"/>
@@ -7947,7 +7948,7 @@
       </c>
       <c r="C46" s="73"/>
       <c r="D46" s="74" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E46" s="74"/>
       <c r="F46" s="74"/>
@@ -8366,12 +8367,19 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="U38:U39"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K38:K39"/>
     <mergeCell ref="R38:S38"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C14:D14"/>
@@ -8388,20 +8396,13 @@
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="L38:L39"/>
     <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="M38:M39"/>
     <mergeCell ref="B34:G34"/>
-    <mergeCell ref="U38:U39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="K38:K39"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -8830,13 +8831,13 @@
         <v>152</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:7">

</xml_diff>

<commit_message>
Import and annotation for java specific is implemented.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiPostSample.xlsx
+++ b/meta/api/BlancoApiPostSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGenerator/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FC2B0A-0F68-0149-8B59-0CCFA1F64DF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9F4277-C9CD-5A4F-B45E-3FAF20CCA75A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="680" windowWidth="21420" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="680" windowWidth="21420" windowHeight="17540" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="236">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2402,6 +2402,28 @@
   </si>
   <si>
     <t>blancoApiSample</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>com.fasterxml.jackson.annotation.JsonProperty</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>電文定義(Java)・インポート</t>
+    <rPh sb="0" eb="4">
+      <t xml:space="preserve">デンブンショリテイギ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>アノテーション(Java)</t>
+    <rPh sb="0" eb="2">
+      <t>ソウショウガタ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>@JsonProperty("field1")</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3645,146 +3667,158 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="60" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3808,44 +3842,32 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4393,7 +4415,7 @@
   </sheetPr>
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:E9"/>
     </sheetView>
   </sheetViews>
@@ -4437,137 +4459,137 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="185" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
+      <c r="B5" s="185"/>
+      <c r="C5" s="185"/>
+      <c r="D5" s="185"/>
+      <c r="E5" s="185"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="95"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="143" t="s">
+      <c r="A6" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="144"/>
-      <c r="C6" s="145"/>
-      <c r="D6" s="140" t="s">
+      <c r="B6" s="183"/>
+      <c r="C6" s="184"/>
+      <c r="D6" s="181" t="s">
         <v>196</v>
       </c>
-      <c r="E6" s="140"/>
+      <c r="E6" s="181"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
       <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="139" t="s">
+      <c r="A7" s="185" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="139"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="140" t="s">
+      <c r="B7" s="185"/>
+      <c r="C7" s="185"/>
+      <c r="D7" s="181" t="s">
         <v>165</v>
       </c>
-      <c r="E7" s="140"/>
+      <c r="E7" s="181"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="139" t="s">
+      <c r="A8" s="185" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="139"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="140" t="s">
+      <c r="B8" s="185"/>
+      <c r="C8" s="185"/>
+      <c r="D8" s="181" t="s">
         <v>231</v>
       </c>
-      <c r="E8" s="140"/>
+      <c r="E8" s="181"/>
       <c r="F8" s="95"/>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="139" t="s">
+      <c r="A9" s="185" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="139"/>
-      <c r="C9" s="139"/>
-      <c r="D9" s="140" t="s">
+      <c r="B9" s="185"/>
+      <c r="C9" s="185"/>
+      <c r="D9" s="181" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="140"/>
+      <c r="E9" s="181"/>
       <c r="F9" s="95"/>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="139" t="s">
+      <c r="A10" s="185" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="139"/>
-      <c r="C10" s="139"/>
-      <c r="D10" s="140"/>
-      <c r="E10" s="140"/>
+      <c r="B10" s="185"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
       <c r="F10" s="95"/>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="139" t="s">
+      <c r="A11" s="185" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="139"/>
-      <c r="C11" s="139"/>
-      <c r="D11" s="140" t="s">
+      <c r="B11" s="185"/>
+      <c r="C11" s="185"/>
+      <c r="D11" s="181" t="s">
         <v>162</v>
       </c>
-      <c r="E11" s="140"/>
+      <c r="E11" s="181"/>
       <c r="F11" s="95"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="146" t="s">
+      <c r="A12" s="144" t="s">
         <v>173</v>
       </c>
-      <c r="B12" s="146"/>
-      <c r="C12" s="146"/>
-      <c r="D12" s="141" t="s">
+      <c r="B12" s="144"/>
+      <c r="C12" s="144"/>
+      <c r="D12" s="165" t="s">
         <v>174</v>
       </c>
-      <c r="E12" s="141"/>
+      <c r="E12" s="165"/>
       <c r="F12" s="95" t="s">
         <v>175</v>
       </c>
       <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="146" t="s">
+      <c r="A13" s="144" t="s">
         <v>211</v>
       </c>
-      <c r="B13" s="146"/>
-      <c r="C13" s="146"/>
-      <c r="D13" s="141" t="s">
+      <c r="B13" s="144"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="165" t="s">
         <v>209</v>
       </c>
-      <c r="E13" s="141"/>
+      <c r="E13" s="165"/>
       <c r="F13" s="95" t="s">
         <v>210</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="146" t="s">
+      <c r="A14" s="144" t="s">
         <v>176</v>
       </c>
-      <c r="B14" s="146"/>
-      <c r="C14" s="146"/>
-      <c r="D14" s="142"/>
-      <c r="E14" s="141"/>
+      <c r="B14" s="144"/>
+      <c r="C14" s="144"/>
+      <c r="D14" s="164"/>
+      <c r="E14" s="165"/>
       <c r="F14" s="54" t="s">
         <v>197</v>
       </c>
@@ -4575,15 +4597,15 @@
       <c r="H14" s="95"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="146" t="s">
+      <c r="A15" s="144" t="s">
         <v>216</v>
       </c>
-      <c r="B15" s="146"/>
-      <c r="C15" s="146"/>
-      <c r="D15" s="142" t="s">
+      <c r="B15" s="144"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="164" t="s">
         <v>214</v>
       </c>
-      <c r="E15" s="141"/>
+      <c r="E15" s="165"/>
       <c r="F15" s="54" t="s">
         <v>219</v>
       </c>
@@ -4591,13 +4613,13 @@
       <c r="H15" s="95"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="146" t="s">
+      <c r="A16" s="144" t="s">
         <v>215</v>
       </c>
-      <c r="B16" s="146"/>
-      <c r="C16" s="146"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="141"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="164"/>
+      <c r="E16" s="165"/>
       <c r="F16" s="54" t="s">
         <v>218</v>
       </c>
@@ -4605,13 +4627,13 @@
       <c r="H16" s="95"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="146" t="s">
+      <c r="A17" s="144" t="s">
         <v>213</v>
       </c>
-      <c r="B17" s="146"/>
-      <c r="C17" s="146"/>
-      <c r="D17" s="142"/>
-      <c r="E17" s="141"/>
+      <c r="B17" s="144"/>
+      <c r="C17" s="144"/>
+      <c r="D17" s="164"/>
+      <c r="E17" s="165"/>
       <c r="F17" s="54" t="s">
         <v>212</v>
       </c>
@@ -4619,19 +4641,19 @@
       <c r="H17" s="95"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="183" t="s">
+      <c r="A18" s="161" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="184"/>
-      <c r="C18" s="185"/>
+      <c r="B18" s="162"/>
+      <c r="C18" s="163"/>
       <c r="D18" s="114"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="169" t="s">
+      <c r="A19" s="145" t="s">
         <v>178</v>
       </c>
-      <c r="B19" s="170"/>
-      <c r="C19" s="171"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="147"/>
       <c r="D19" s="100"/>
       <c r="E19" t="s">
         <v>179</v>
@@ -4649,15 +4671,15 @@
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="180" t="s">
+      <c r="A21" s="158" t="s">
         <v>187</v>
       </c>
-      <c r="B21" s="181"/>
-      <c r="C21" s="181"/>
-      <c r="D21" s="181"/>
-      <c r="E21" s="181"/>
-      <c r="F21" s="181"/>
-      <c r="G21" s="182"/>
+      <c r="B21" s="159"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="160"/>
       <c r="H21" s="1" t="s">
         <v>222</v>
       </c>
@@ -4708,28 +4730,28 @@
       <c r="C25"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="179" t="s">
+      <c r="A26" s="157" t="s">
         <v>188</v>
       </c>
-      <c r="B26" s="179"/>
-      <c r="C26" s="179"/>
-      <c r="D26" s="179"/>
-      <c r="E26" s="179"/>
-      <c r="F26" s="179"/>
-      <c r="G26" s="179"/>
+      <c r="B26" s="157"/>
+      <c r="C26" s="157"/>
+      <c r="D26" s="157"/>
+      <c r="E26" s="157"/>
+      <c r="F26" s="157"/>
+      <c r="G26" s="157"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="173" t="s">
+      <c r="B27" s="151" t="s">
         <v>182</v>
       </c>
-      <c r="C27" s="174"/>
-      <c r="D27" s="174"/>
-      <c r="E27" s="174"/>
-      <c r="F27" s="174"/>
-      <c r="G27" s="175"/>
+      <c r="C27" s="152"/>
+      <c r="D27" s="152"/>
+      <c r="E27" s="152"/>
+      <c r="F27" s="152"/>
+      <c r="G27" s="153"/>
       <c r="H27" s="105"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -4740,12 +4762,12 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="116"/>
-      <c r="B28" s="157"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
+      <c r="B28" s="168"/>
+      <c r="C28" s="168"/>
+      <c r="D28" s="168"/>
+      <c r="E28" s="168"/>
+      <c r="F28" s="168"/>
+      <c r="G28" s="168"/>
       <c r="H28" s="112"/>
       <c r="I28" s="112"/>
       <c r="J28" s="112"/>
@@ -4756,12 +4778,12 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="117"/>
-      <c r="B29" s="159"/>
-      <c r="C29" s="159"/>
-      <c r="D29" s="159"/>
-      <c r="E29" s="159"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="159"/>
+      <c r="B29" s="169"/>
+      <c r="C29" s="169"/>
+      <c r="D29" s="169"/>
+      <c r="E29" s="169"/>
+      <c r="F29" s="169"/>
+      <c r="G29" s="169"/>
       <c r="H29" s="112"/>
       <c r="I29" s="112"/>
       <c r="J29" s="112"/>
@@ -4772,12 +4794,12 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="118"/>
-      <c r="B30" s="161"/>
-      <c r="C30" s="161"/>
-      <c r="D30" s="161"/>
-      <c r="E30" s="161"/>
-      <c r="F30" s="161"/>
-      <c r="G30" s="161"/>
+      <c r="B30" s="170"/>
+      <c r="C30" s="170"/>
+      <c r="D30" s="170"/>
+      <c r="E30" s="170"/>
+      <c r="F30" s="170"/>
+      <c r="G30" s="170"/>
       <c r="H30" s="112"/>
       <c r="I30" s="112"/>
       <c r="J30" s="112"/>
@@ -4790,28 +4812,28 @@
       <c r="C31"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="176" t="s">
+      <c r="A32" s="154" t="s">
         <v>189</v>
       </c>
-      <c r="B32" s="177"/>
-      <c r="C32" s="177"/>
-      <c r="D32" s="177"/>
-      <c r="E32" s="177"/>
-      <c r="F32" s="177"/>
-      <c r="G32" s="178"/>
+      <c r="B32" s="155"/>
+      <c r="C32" s="155"/>
+      <c r="D32" s="155"/>
+      <c r="E32" s="155"/>
+      <c r="F32" s="155"/>
+      <c r="G32" s="156"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="153" t="s">
+      <c r="B33" s="174" t="s">
         <v>183</v>
       </c>
-      <c r="C33" s="153"/>
-      <c r="D33" s="153"/>
-      <c r="E33" s="153"/>
-      <c r="F33" s="153"/>
-      <c r="G33" s="153"/>
+      <c r="C33" s="174"/>
+      <c r="D33" s="174"/>
+      <c r="E33" s="174"/>
+      <c r="F33" s="174"/>
+      <c r="G33" s="174"/>
       <c r="H33" s="105"/>
       <c r="I33" s="105"/>
       <c r="J33" s="105"/>
@@ -4824,14 +4846,14 @@
       <c r="A34" s="116">
         <v>1</v>
       </c>
-      <c r="B34" s="154" t="s">
+      <c r="B34" s="175" t="s">
         <v>217</v>
       </c>
-      <c r="C34" s="154"/>
-      <c r="D34" s="154"/>
-      <c r="E34" s="154"/>
-      <c r="F34" s="154"/>
-      <c r="G34" s="154"/>
+      <c r="C34" s="175"/>
+      <c r="D34" s="175"/>
+      <c r="E34" s="175"/>
+      <c r="F34" s="175"/>
+      <c r="G34" s="175"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -4842,12 +4864,12 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="117"/>
-      <c r="B35" s="155"/>
-      <c r="C35" s="155"/>
-      <c r="D35" s="155"/>
-      <c r="E35" s="155"/>
-      <c r="F35" s="155"/>
-      <c r="G35" s="155"/>
+      <c r="B35" s="176"/>
+      <c r="C35" s="176"/>
+      <c r="D35" s="176"/>
+      <c r="E35" s="176"/>
+      <c r="F35" s="176"/>
+      <c r="G35" s="176"/>
       <c r="H35" s="112"/>
       <c r="I35" s="112"/>
       <c r="J35" s="112"/>
@@ -4858,12 +4880,12 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="118"/>
-      <c r="B36" s="156"/>
-      <c r="C36" s="156"/>
-      <c r="D36" s="156"/>
-      <c r="E36" s="156"/>
-      <c r="F36" s="156"/>
-      <c r="G36" s="156"/>
+      <c r="B36" s="177"/>
+      <c r="C36" s="177"/>
+      <c r="D36" s="177"/>
+      <c r="E36" s="177"/>
+      <c r="F36" s="177"/>
+      <c r="G36" s="177"/>
       <c r="H36" s="112"/>
       <c r="I36" s="112"/>
       <c r="J36" s="112"/>
@@ -4888,28 +4910,28 @@
       <c r="M37"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="176" t="s">
+      <c r="A38" s="154" t="s">
         <v>190</v>
       </c>
-      <c r="B38" s="177"/>
-      <c r="C38" s="177"/>
-      <c r="D38" s="177"/>
-      <c r="E38" s="177"/>
-      <c r="F38" s="177"/>
-      <c r="G38" s="178"/>
+      <c r="B38" s="155"/>
+      <c r="C38" s="155"/>
+      <c r="D38" s="155"/>
+      <c r="E38" s="155"/>
+      <c r="F38" s="155"/>
+      <c r="G38" s="156"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="153" t="s">
+      <c r="B39" s="174" t="s">
         <v>185</v>
       </c>
-      <c r="C39" s="153"/>
-      <c r="D39" s="153"/>
-      <c r="E39" s="153"/>
-      <c r="F39" s="153"/>
-      <c r="G39" s="153"/>
+      <c r="C39" s="174"/>
+      <c r="D39" s="174"/>
+      <c r="E39" s="174"/>
+      <c r="F39" s="174"/>
+      <c r="G39" s="174"/>
       <c r="H39" s="105"/>
       <c r="I39" s="105"/>
       <c r="J39" s="105"/>
@@ -4920,12 +4942,12 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="116"/>
-      <c r="B40" s="157"/>
-      <c r="C40" s="157"/>
-      <c r="D40" s="157"/>
-      <c r="E40" s="157"/>
-      <c r="F40" s="157"/>
-      <c r="G40" s="158"/>
+      <c r="B40" s="168"/>
+      <c r="C40" s="168"/>
+      <c r="D40" s="168"/>
+      <c r="E40" s="168"/>
+      <c r="F40" s="168"/>
+      <c r="G40" s="178"/>
       <c r="H40" s="112"/>
       <c r="I40" s="112"/>
       <c r="J40" s="112"/>
@@ -4936,12 +4958,12 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="117"/>
-      <c r="B41" s="159"/>
-      <c r="C41" s="159"/>
-      <c r="D41" s="159"/>
-      <c r="E41" s="159"/>
-      <c r="F41" s="159"/>
-      <c r="G41" s="160"/>
+      <c r="B41" s="169"/>
+      <c r="C41" s="169"/>
+      <c r="D41" s="169"/>
+      <c r="E41" s="169"/>
+      <c r="F41" s="169"/>
+      <c r="G41" s="179"/>
       <c r="H41" s="112"/>
       <c r="I41" s="112"/>
       <c r="J41" s="112"/>
@@ -4952,12 +4974,12 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="118"/>
-      <c r="B42" s="161"/>
-      <c r="C42" s="161"/>
-      <c r="D42" s="161"/>
-      <c r="E42" s="161"/>
-      <c r="F42" s="161"/>
-      <c r="G42" s="162"/>
+      <c r="B42" s="170"/>
+      <c r="C42" s="170"/>
+      <c r="D42" s="170"/>
+      <c r="E42" s="170"/>
+      <c r="F42" s="170"/>
+      <c r="G42" s="180"/>
       <c r="H42" s="112"/>
       <c r="I42" s="112"/>
       <c r="J42" s="112"/>
@@ -4992,254 +5014,267 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="166" t="s">
+      <c r="A45" s="141" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="172"/>
-      <c r="C45" s="166" t="s">
+      <c r="B45" s="148"/>
+      <c r="C45" s="141" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="167"/>
-      <c r="E45" s="168"/>
+      <c r="D45" s="142"/>
+      <c r="E45" s="143"/>
       <c r="F45" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="163"/>
-      <c r="B46" s="165"/>
-      <c r="C46" s="163"/>
-      <c r="D46" s="164"/>
-      <c r="E46" s="165"/>
+      <c r="A46" s="149"/>
+      <c r="B46" s="150"/>
+      <c r="C46" s="149"/>
+      <c r="D46" s="171"/>
+      <c r="E46" s="150"/>
       <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="147"/>
-      <c r="B47" s="149"/>
-      <c r="C47" s="147"/>
-      <c r="D47" s="148"/>
-      <c r="E47" s="149"/>
+      <c r="A47" s="139"/>
+      <c r="B47" s="140"/>
+      <c r="C47" s="139"/>
+      <c r="D47" s="172"/>
+      <c r="E47" s="140"/>
       <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="147"/>
-      <c r="B48" s="149"/>
-      <c r="C48" s="147"/>
-      <c r="D48" s="148"/>
-      <c r="E48" s="149"/>
+      <c r="A48" s="139"/>
+      <c r="B48" s="140"/>
+      <c r="C48" s="139"/>
+      <c r="D48" s="172"/>
+      <c r="E48" s="140"/>
       <c r="F48" s="49"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="147"/>
-      <c r="B49" s="149"/>
-      <c r="C49" s="147"/>
-      <c r="D49" s="148"/>
-      <c r="E49" s="149"/>
+      <c r="A49" s="139"/>
+      <c r="B49" s="140"/>
+      <c r="C49" s="139"/>
+      <c r="D49" s="172"/>
+      <c r="E49" s="140"/>
       <c r="F49" s="49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="147"/>
-      <c r="B50" s="149"/>
-      <c r="C50" s="147"/>
-      <c r="D50" s="148"/>
-      <c r="E50" s="149"/>
+      <c r="A50" s="139"/>
+      <c r="B50" s="140"/>
+      <c r="C50" s="139"/>
+      <c r="D50" s="172"/>
+      <c r="E50" s="140"/>
       <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="147"/>
-      <c r="B51" s="149"/>
-      <c r="C51" s="147"/>
-      <c r="D51" s="148"/>
-      <c r="E51" s="149"/>
+      <c r="A51" s="139"/>
+      <c r="B51" s="140"/>
+      <c r="C51" s="139"/>
+      <c r="D51" s="172"/>
+      <c r="E51" s="140"/>
       <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="147"/>
-      <c r="B52" s="149"/>
-      <c r="C52" s="147"/>
-      <c r="D52" s="148"/>
-      <c r="E52" s="149"/>
+      <c r="A52" s="139"/>
+      <c r="B52" s="140"/>
+      <c r="C52" s="139"/>
+      <c r="D52" s="172"/>
+      <c r="E52" s="140"/>
       <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="147"/>
-      <c r="B53" s="149"/>
-      <c r="C53" s="147"/>
-      <c r="D53" s="148"/>
-      <c r="E53" s="149"/>
+      <c r="A53" s="139"/>
+      <c r="B53" s="140"/>
+      <c r="C53" s="139"/>
+      <c r="D53" s="172"/>
+      <c r="E53" s="140"/>
       <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="147"/>
-      <c r="B54" s="149"/>
-      <c r="C54" s="147"/>
-      <c r="D54" s="148"/>
-      <c r="E54" s="149"/>
+      <c r="A54" s="139"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="139"/>
+      <c r="D54" s="172"/>
+      <c r="E54" s="140"/>
       <c r="F54" s="49"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="147"/>
-      <c r="B55" s="149"/>
-      <c r="C55" s="147"/>
-      <c r="D55" s="148"/>
-      <c r="E55" s="149"/>
+      <c r="A55" s="139"/>
+      <c r="B55" s="140"/>
+      <c r="C55" s="139"/>
+      <c r="D55" s="172"/>
+      <c r="E55" s="140"/>
       <c r="F55" s="49"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="147"/>
-      <c r="B56" s="149"/>
-      <c r="C56" s="147"/>
-      <c r="D56" s="148"/>
-      <c r="E56" s="149"/>
+      <c r="A56" s="139"/>
+      <c r="B56" s="140"/>
+      <c r="C56" s="139"/>
+      <c r="D56" s="172"/>
+      <c r="E56" s="140"/>
       <c r="F56" s="49"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="147"/>
-      <c r="B57" s="149"/>
-      <c r="C57" s="147"/>
-      <c r="D57" s="148"/>
-      <c r="E57" s="149"/>
+      <c r="A57" s="139"/>
+      <c r="B57" s="140"/>
+      <c r="C57" s="139"/>
+      <c r="D57" s="172"/>
+      <c r="E57" s="140"/>
       <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="147"/>
-      <c r="B58" s="149"/>
-      <c r="C58" s="147"/>
-      <c r="D58" s="148"/>
-      <c r="E58" s="149"/>
+      <c r="A58" s="139"/>
+      <c r="B58" s="140"/>
+      <c r="C58" s="139"/>
+      <c r="D58" s="172"/>
+      <c r="E58" s="140"/>
       <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="147"/>
-      <c r="B59" s="149"/>
-      <c r="C59" s="147"/>
-      <c r="D59" s="148"/>
-      <c r="E59" s="149"/>
+      <c r="A59" s="139"/>
+      <c r="B59" s="140"/>
+      <c r="C59" s="139"/>
+      <c r="D59" s="172"/>
+      <c r="E59" s="140"/>
       <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="147"/>
-      <c r="B60" s="149"/>
-      <c r="C60" s="147"/>
-      <c r="D60" s="148"/>
-      <c r="E60" s="149"/>
+      <c r="A60" s="139"/>
+      <c r="B60" s="140"/>
+      <c r="C60" s="139"/>
+      <c r="D60" s="172"/>
+      <c r="E60" s="140"/>
       <c r="F60" s="49"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="147"/>
-      <c r="B61" s="149"/>
-      <c r="C61" s="147"/>
-      <c r="D61" s="148"/>
-      <c r="E61" s="149"/>
+      <c r="A61" s="139"/>
+      <c r="B61" s="140"/>
+      <c r="C61" s="139"/>
+      <c r="D61" s="172"/>
+      <c r="E61" s="140"/>
       <c r="F61" s="49"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="147"/>
-      <c r="B62" s="149"/>
-      <c r="C62" s="147"/>
-      <c r="D62" s="148"/>
-      <c r="E62" s="149"/>
+      <c r="A62" s="139"/>
+      <c r="B62" s="140"/>
+      <c r="C62" s="139"/>
+      <c r="D62" s="172"/>
+      <c r="E62" s="140"/>
       <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="147"/>
-      <c r="B63" s="149"/>
-      <c r="C63" s="147"/>
-      <c r="D63" s="148"/>
-      <c r="E63" s="149"/>
+      <c r="A63" s="139"/>
+      <c r="B63" s="140"/>
+      <c r="C63" s="139"/>
+      <c r="D63" s="172"/>
+      <c r="E63" s="140"/>
       <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="147"/>
-      <c r="B64" s="149"/>
-      <c r="C64" s="147"/>
-      <c r="D64" s="148"/>
-      <c r="E64" s="149"/>
+      <c r="A64" s="139"/>
+      <c r="B64" s="140"/>
+      <c r="C64" s="139"/>
+      <c r="D64" s="172"/>
+      <c r="E64" s="140"/>
       <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="147"/>
-      <c r="B65" s="149"/>
-      <c r="C65" s="147"/>
-      <c r="D65" s="148"/>
-      <c r="E65" s="149"/>
+      <c r="A65" s="139"/>
+      <c r="B65" s="140"/>
+      <c r="C65" s="139"/>
+      <c r="D65" s="172"/>
+      <c r="E65" s="140"/>
       <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="147"/>
-      <c r="B66" s="149"/>
-      <c r="C66" s="147"/>
-      <c r="D66" s="148"/>
-      <c r="E66" s="149"/>
+      <c r="A66" s="139"/>
+      <c r="B66" s="140"/>
+      <c r="C66" s="139"/>
+      <c r="D66" s="172"/>
+      <c r="E66" s="140"/>
       <c r="F66" s="49"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="147"/>
-      <c r="B67" s="149"/>
-      <c r="C67" s="147"/>
-      <c r="D67" s="148"/>
-      <c r="E67" s="149"/>
+      <c r="A67" s="139"/>
+      <c r="B67" s="140"/>
+      <c r="C67" s="139"/>
+      <c r="D67" s="172"/>
+      <c r="E67" s="140"/>
       <c r="F67" s="49"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="147"/>
-      <c r="B68" s="149"/>
-      <c r="C68" s="147"/>
-      <c r="D68" s="148"/>
-      <c r="E68" s="149"/>
+      <c r="A68" s="139"/>
+      <c r="B68" s="140"/>
+      <c r="C68" s="139"/>
+      <c r="D68" s="172"/>
+      <c r="E68" s="140"/>
       <c r="F68" s="49"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="147"/>
-      <c r="B69" s="149"/>
-      <c r="C69" s="147"/>
-      <c r="D69" s="148"/>
-      <c r="E69" s="149"/>
+      <c r="A69" s="139"/>
+      <c r="B69" s="140"/>
+      <c r="C69" s="139"/>
+      <c r="D69" s="172"/>
+      <c r="E69" s="140"/>
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="150"/>
-      <c r="B70" s="152"/>
-      <c r="C70" s="150"/>
-      <c r="D70" s="151"/>
-      <c r="E70" s="152"/>
+      <c r="A70" s="166"/>
+      <c r="B70" s="167"/>
+      <c r="C70" s="166"/>
+      <c r="D70" s="173"/>
+      <c r="E70" s="167"/>
       <c r="F70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="A69:B69"/>
@@ -5256,52 +5291,39 @@
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="C53:E53"/>
     <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="1">
@@ -5334,10 +5356,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z66"/>
+  <dimension ref="A1:Z72"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="J29" workbookViewId="0">
+      <selection activeCell="V47" sqref="V47:V48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5360,7 +5382,7 @@
     <col min="19" max="19" width="6.83203125" style="1" customWidth="1"/>
     <col min="20" max="20" width="9" style="1" customWidth="1"/>
     <col min="21" max="21" width="16.6640625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="6.83203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.6640625" style="1" customWidth="1"/>
     <col min="24" max="24" width="43.5" style="1" customWidth="1"/>
     <col min="25" max="25" width="11.33203125" style="1" customWidth="1"/>
@@ -5375,7 +5397,7 @@
     <col min="34" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="19">
+    <row r="1" spans="1:22" ht="19">
       <c r="A1" s="18" t="s">
         <v>23</v>
       </c>
@@ -5383,17 +5405,17 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:22">
       <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:22">
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:22">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -5408,7 +5430,7 @@
       <c r="N5" s="28"/>
       <c r="O5" s="28"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:22">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -5426,7 +5448,7 @@
       <c r="N6" s="28"/>
       <c r="O6" s="28"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:22">
       <c r="A7" s="4" t="s">
         <v>81</v>
       </c>
@@ -5447,7 +5469,7 @@
       <c r="R7" s="54"/>
       <c r="S7"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:22">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -5467,7 +5489,7 @@
       <c r="N8" s="28"/>
       <c r="O8" s="28"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:22">
       <c r="A9" s="4" t="s">
         <v>155</v>
       </c>
@@ -5484,7 +5506,7 @@
       <c r="N9" s="28"/>
       <c r="O9" s="28"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:22">
       <c r="A10" s="56" t="s">
         <v>156</v>
       </c>
@@ -5498,7 +5520,7 @@
       <c r="N10" s="28"/>
       <c r="O10" s="28"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:22">
       <c r="A11" s="56" t="s">
         <v>157</v>
       </c>
@@ -5512,7 +5534,7 @@
       <c r="N11" s="28"/>
       <c r="O11" s="28"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:22">
       <c r="A12" s="56" t="s">
         <v>158</v>
       </c>
@@ -5526,7 +5548,7 @@
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:22">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -5537,7 +5559,7 @@
       <c r="F13" s="54"/>
       <c r="G13" s="54"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:22">
       <c r="A14" s="4" t="s">
         <v>99</v>
       </c>
@@ -5553,16 +5575,17 @@
       <c r="J14"/>
       <c r="K14"/>
       <c r="L14"/>
-    </row>
-    <row r="15" spans="1:19">
+      <c r="V14"/>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="122" t="s">
         <v>173</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="141" t="s">
+      <c r="C15" s="165" t="s">
         <v>174</v>
       </c>
-      <c r="D15" s="141"/>
+      <c r="D15" s="165"/>
       <c r="E15" s="95" t="s">
         <v>175</v>
       </c>
@@ -5571,16 +5594,17 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15"/>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="V15"/>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="122" t="s">
         <v>225</v>
       </c>
       <c r="B16" s="122"/>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="164" t="s">
         <v>229</v>
       </c>
-      <c r="D16" s="141"/>
+      <c r="D16" s="165"/>
       <c r="E16" s="55" t="s">
         <v>226</v>
       </c>
@@ -5594,16 +5618,17 @@
       <c r="M16" s="95"/>
       <c r="N16" s="95"/>
       <c r="O16" s="95"/>
+      <c r="V16"/>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="122" t="s">
         <v>176</v>
       </c>
       <c r="B17" s="122"/>
-      <c r="C17" s="141" t="s">
+      <c r="C17" s="165" t="s">
         <v>177</v>
       </c>
-      <c r="D17" s="141"/>
+      <c r="D17" s="165"/>
       <c r="E17" s="55"/>
       <c r="F17" s="55"/>
       <c r="G17" s="54"/>
@@ -5615,8 +5640,8 @@
         <v>227</v>
       </c>
       <c r="B18" s="122"/>
-      <c r="C18" s="142"/>
-      <c r="D18" s="141"/>
+      <c r="C18" s="164"/>
+      <c r="D18" s="165"/>
       <c r="E18" s="55" t="s">
         <v>228</v>
       </c>
@@ -5630,6 +5655,7 @@
       <c r="M18" s="95"/>
       <c r="N18" s="95"/>
       <c r="O18" s="95"/>
+      <c r="V18"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="123" t="s">
@@ -5656,6 +5682,7 @@
       <c r="Q19"/>
       <c r="R19"/>
       <c r="S19"/>
+      <c r="V19"/>
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="6"/>
@@ -5664,34 +5691,36 @@
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
+      <c r="V20"/>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" s="179" t="s">
+      <c r="A21" s="157" t="s">
         <v>191</v>
       </c>
-      <c r="B21" s="179"/>
-      <c r="C21" s="179"/>
-      <c r="D21" s="179"/>
-      <c r="E21" s="179"/>
-      <c r="F21" s="179"/>
-      <c r="G21" s="179"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
+      <c r="V21"/>
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="173" t="s">
+      <c r="B22" s="151" t="s">
         <v>182</v>
       </c>
-      <c r="C22" s="174"/>
-      <c r="D22" s="174"/>
-      <c r="E22" s="174"/>
-      <c r="F22" s="174"/>
-      <c r="G22" s="175"/>
+      <c r="C22" s="152"/>
+      <c r="D22" s="152"/>
+      <c r="E22" s="152"/>
+      <c r="F22" s="152"/>
+      <c r="G22" s="153"/>
       <c r="H22" s="105"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -5705,16 +5734,16 @@
       <c r="R22" s="105"/>
       <c r="S22" s="105"/>
       <c r="U22" s="111"/>
-      <c r="V22" s="111"/>
+      <c r="V22"/>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="116"/>
-      <c r="B23" s="157"/>
-      <c r="C23" s="157"/>
-      <c r="D23" s="157"/>
-      <c r="E23" s="157"/>
-      <c r="F23" s="157"/>
-      <c r="G23" s="157"/>
+      <c r="B23" s="168"/>
+      <c r="C23" s="168"/>
+      <c r="D23" s="168"/>
+      <c r="E23" s="168"/>
+      <c r="F23" s="168"/>
+      <c r="G23" s="168"/>
       <c r="H23" s="112"/>
       <c r="I23"/>
       <c r="J23"/>
@@ -5732,12 +5761,12 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="117"/>
-      <c r="B24" s="159"/>
-      <c r="C24" s="159"/>
-      <c r="D24" s="159"/>
-      <c r="E24" s="159"/>
-      <c r="F24" s="159"/>
-      <c r="G24" s="159"/>
+      <c r="B24" s="169"/>
+      <c r="C24" s="169"/>
+      <c r="D24" s="169"/>
+      <c r="E24" s="169"/>
+      <c r="F24" s="169"/>
+      <c r="G24" s="169"/>
       <c r="H24" s="112"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -5755,12 +5784,12 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="118"/>
-      <c r="B25" s="161"/>
-      <c r="C25" s="161"/>
-      <c r="D25" s="161"/>
-      <c r="E25" s="161"/>
-      <c r="F25" s="161"/>
-      <c r="G25" s="161"/>
+      <c r="B25" s="170"/>
+      <c r="C25" s="170"/>
+      <c r="D25" s="170"/>
+      <c r="E25" s="170"/>
+      <c r="F25" s="170"/>
+      <c r="G25" s="170"/>
       <c r="H25" s="112"/>
       <c r="M25" s="112"/>
       <c r="N25" s="112"/>
@@ -5770,7 +5799,6 @@
       <c r="R25" s="112"/>
       <c r="T25"/>
       <c r="U25"/>
-      <c r="V25"/>
     </row>
     <row r="26" spans="1:22">
       <c r="C26"/>
@@ -5778,34 +5806,36 @@
       <c r="J26" s="105"/>
       <c r="K26" s="105"/>
       <c r="L26" s="105"/>
+      <c r="V26" s="105"/>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="176" t="s">
+      <c r="A27" s="154" t="s">
         <v>192</v>
       </c>
-      <c r="B27" s="177"/>
-      <c r="C27" s="177"/>
-      <c r="D27" s="177"/>
-      <c r="E27" s="177"/>
-      <c r="F27" s="177"/>
-      <c r="G27" s="178"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="155"/>
+      <c r="D27" s="155"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="155"/>
+      <c r="G27" s="156"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
       <c r="K27" s="105"/>
       <c r="L27" s="105"/>
+      <c r="V27" s="105"/>
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="153" t="s">
+      <c r="B28" s="174" t="s">
         <v>183</v>
       </c>
-      <c r="C28" s="153"/>
-      <c r="D28" s="153"/>
-      <c r="E28" s="153"/>
-      <c r="F28" s="153"/>
-      <c r="G28" s="153"/>
+      <c r="C28" s="174"/>
+      <c r="D28" s="174"/>
+      <c r="E28" s="174"/>
+      <c r="F28" s="174"/>
+      <c r="G28" s="174"/>
       <c r="H28" s="105"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -5819,20 +5849,20 @@
       <c r="R28" s="105"/>
       <c r="S28" s="105"/>
       <c r="U28" s="111"/>
-      <c r="V28" s="111"/>
+      <c r="V28" s="105"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="116">
         <v>1</v>
       </c>
-      <c r="B29" s="154" t="s">
+      <c r="B29" s="175" t="s">
         <v>224</v>
       </c>
-      <c r="C29" s="154"/>
-      <c r="D29" s="154"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
+      <c r="C29" s="175"/>
+      <c r="D29" s="175"/>
+      <c r="E29" s="175"/>
+      <c r="F29" s="175"/>
+      <c r="G29" s="175"/>
       <c r="H29" s="112"/>
       <c r="I29"/>
       <c r="J29"/>
@@ -5850,12 +5880,14 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="117"/>
-      <c r="B30" s="155"/>
-      <c r="C30" s="155"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="155"/>
+      <c r="B30" s="176" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" s="176"/>
+      <c r="D30" s="176"/>
+      <c r="E30" s="176"/>
+      <c r="F30" s="176"/>
+      <c r="G30" s="176"/>
       <c r="H30" s="112"/>
       <c r="M30" s="112"/>
       <c r="N30" s="112"/>
@@ -5865,16 +5897,15 @@
       <c r="R30" s="112"/>
       <c r="T30"/>
       <c r="U30"/>
-      <c r="V30"/>
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="118"/>
-      <c r="B31" s="156"/>
-      <c r="C31" s="156"/>
-      <c r="D31" s="156"/>
-      <c r="E31" s="156"/>
-      <c r="F31" s="156"/>
-      <c r="G31" s="156"/>
+      <c r="B31" s="177"/>
+      <c r="C31" s="177"/>
+      <c r="D31" s="177"/>
+      <c r="E31" s="177"/>
+      <c r="F31" s="177"/>
+      <c r="G31" s="177"/>
       <c r="H31" s="112"/>
       <c r="I31" s="105"/>
       <c r="J31" s="105"/>
@@ -5888,7 +5919,7 @@
       <c r="R31" s="112"/>
       <c r="T31"/>
       <c r="U31"/>
-      <c r="V31"/>
+      <c r="V31" s="105"/>
     </row>
     <row r="32" spans="1:22">
       <c r="A32"/>
@@ -5911,39 +5942,41 @@
       <c r="R32"/>
       <c r="S32"/>
       <c r="T32"/>
+      <c r="V32" s="112"/>
     </row>
     <row r="33" spans="1:26">
-      <c r="A33" s="176" t="s">
-        <v>193</v>
-      </c>
-      <c r="B33" s="177"/>
-      <c r="C33" s="177"/>
-      <c r="D33" s="177"/>
-      <c r="E33" s="177"/>
-      <c r="F33" s="177"/>
-      <c r="G33" s="178"/>
-      <c r="I33" s="112"/>
-      <c r="J33" s="112"/>
-      <c r="K33" s="112"/>
-      <c r="L33" s="112"/>
+      <c r="A33" s="154" t="s">
+        <v>233</v>
+      </c>
+      <c r="B33" s="155"/>
+      <c r="C33" s="155"/>
+      <c r="D33" s="155"/>
+      <c r="E33" s="155"/>
+      <c r="F33" s="155"/>
+      <c r="G33" s="156"/>
+      <c r="I33" s="105"/>
+      <c r="J33" s="105"/>
+      <c r="K33" s="105"/>
+      <c r="L33" s="105"/>
+      <c r="V33" s="105"/>
     </row>
     <row r="34" spans="1:26">
       <c r="A34" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="153" t="s">
-        <v>185</v>
-      </c>
-      <c r="C34" s="153"/>
-      <c r="D34" s="153"/>
-      <c r="E34" s="153"/>
-      <c r="F34" s="153"/>
-      <c r="G34" s="153"/>
+      <c r="B34" s="174" t="s">
+        <v>183</v>
+      </c>
+      <c r="C34" s="174"/>
+      <c r="D34" s="174"/>
+      <c r="E34" s="174"/>
+      <c r="F34" s="174"/>
+      <c r="G34" s="174"/>
       <c r="H34" s="105"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="112"/>
-      <c r="K34" s="112"/>
-      <c r="L34" s="112"/>
+      <c r="I34" s="105"/>
+      <c r="J34" s="105"/>
+      <c r="K34" s="105"/>
+      <c r="L34" s="105"/>
       <c r="M34" s="105"/>
       <c r="N34" s="105"/>
       <c r="O34" s="105"/>
@@ -5952,16 +5985,20 @@
       <c r="R34" s="105"/>
       <c r="S34" s="105"/>
       <c r="U34" s="111"/>
-      <c r="V34" s="111"/>
+      <c r="V34" s="105"/>
     </row>
     <row r="35" spans="1:26">
-      <c r="A35" s="116"/>
-      <c r="B35" s="157"/>
-      <c r="C35" s="157"/>
-      <c r="D35" s="157"/>
-      <c r="E35" s="157"/>
-      <c r="F35" s="157"/>
-      <c r="G35" s="158"/>
+      <c r="A35" s="116">
+        <v>1</v>
+      </c>
+      <c r="B35" s="175" t="s">
+        <v>232</v>
+      </c>
+      <c r="C35" s="175"/>
+      <c r="D35" s="175"/>
+      <c r="E35" s="175"/>
+      <c r="F35" s="175"/>
+      <c r="G35" s="175"/>
       <c r="H35" s="112"/>
       <c r="I35"/>
       <c r="J35"/>
@@ -5979,12 +6016,12 @@
     </row>
     <row r="36" spans="1:26">
       <c r="A36" s="117"/>
-      <c r="B36" s="159"/>
-      <c r="C36" s="159"/>
-      <c r="D36" s="159"/>
-      <c r="E36" s="159"/>
-      <c r="F36" s="159"/>
-      <c r="G36" s="160"/>
+      <c r="B36" s="176"/>
+      <c r="C36" s="176"/>
+      <c r="D36" s="176"/>
+      <c r="E36" s="176"/>
+      <c r="F36" s="176"/>
+      <c r="G36" s="176"/>
       <c r="H36" s="112"/>
       <c r="M36" s="112"/>
       <c r="N36" s="112"/>
@@ -5994,17 +6031,20 @@
       <c r="R36" s="112"/>
       <c r="T36"/>
       <c r="U36"/>
-      <c r="V36"/>
     </row>
     <row r="37" spans="1:26">
       <c r="A37" s="118"/>
-      <c r="B37" s="161"/>
-      <c r="C37" s="161"/>
-      <c r="D37" s="161"/>
-      <c r="E37" s="161"/>
-      <c r="F37" s="161"/>
-      <c r="G37" s="162"/>
+      <c r="B37" s="177"/>
+      <c r="C37" s="177"/>
+      <c r="D37" s="177"/>
+      <c r="E37" s="177"/>
+      <c r="F37" s="177"/>
+      <c r="G37" s="177"/>
       <c r="H37" s="112"/>
+      <c r="I37" s="105"/>
+      <c r="J37" s="105"/>
+      <c r="K37" s="105"/>
+      <c r="L37" s="105"/>
       <c r="M37" s="112"/>
       <c r="N37" s="112"/>
       <c r="O37" s="112"/>
@@ -6013,7 +6053,7 @@
       <c r="R37" s="112"/>
       <c r="T37"/>
       <c r="U37"/>
-      <c r="V37"/>
+      <c r="V37" s="105"/>
     </row>
     <row r="38" spans="1:26">
       <c r="A38"/>
@@ -6024,6 +6064,10 @@
       <c r="F38"/>
       <c r="G38"/>
       <c r="H38"/>
+      <c r="I38" s="112"/>
+      <c r="J38" s="112"/>
+      <c r="K38" s="112"/>
+      <c r="L38" s="112"/>
       <c r="M38"/>
       <c r="N38"/>
       <c r="O38"/>
@@ -6032,514 +6076,489 @@
       <c r="R38"/>
       <c r="S38"/>
       <c r="T38"/>
+      <c r="V38" s="112"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="6"/>
+      <c r="A39" s="154" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="155"/>
+      <c r="C39" s="155"/>
+      <c r="D39" s="155"/>
+      <c r="E39" s="155"/>
+      <c r="F39" s="155"/>
+      <c r="G39" s="156"/>
+      <c r="I39" s="112"/>
+      <c r="J39" s="112"/>
+      <c r="K39" s="112"/>
+      <c r="L39" s="112"/>
+      <c r="V39" s="112"/>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="174" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="174"/>
+      <c r="D40" s="174"/>
+      <c r="E40" s="174"/>
+      <c r="F40" s="174"/>
+      <c r="G40" s="174"/>
+      <c r="H40" s="105"/>
+      <c r="I40" s="112"/>
+      <c r="J40" s="112"/>
+      <c r="K40" s="112"/>
+      <c r="L40" s="112"/>
+      <c r="M40" s="105"/>
+      <c r="N40" s="105"/>
+      <c r="O40" s="105"/>
+      <c r="P40" s="105"/>
+      <c r="Q40" s="105"/>
+      <c r="R40" s="105"/>
+      <c r="S40" s="105"/>
+      <c r="U40" s="111"/>
+      <c r="V40" s="112"/>
+    </row>
+    <row r="41" spans="1:26">
+      <c r="A41" s="116"/>
+      <c r="B41" s="168"/>
+      <c r="C41" s="168"/>
+      <c r="D41" s="168"/>
+      <c r="E41" s="168"/>
+      <c r="F41" s="168"/>
+      <c r="G41" s="178"/>
+      <c r="H41" s="112"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41" s="112"/>
+      <c r="N41" s="112"/>
+      <c r="O41" s="112"/>
+      <c r="P41" s="112"/>
+      <c r="Q41" s="112"/>
+      <c r="R41" s="112"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+    </row>
+    <row r="42" spans="1:26">
+      <c r="A42" s="117"/>
+      <c r="B42" s="169"/>
+      <c r="C42" s="169"/>
+      <c r="D42" s="169"/>
+      <c r="E42" s="169"/>
+      <c r="F42" s="169"/>
+      <c r="G42" s="179"/>
+      <c r="H42" s="112"/>
+      <c r="M42" s="112"/>
+      <c r="N42" s="112"/>
+      <c r="O42" s="112"/>
+      <c r="P42" s="112"/>
+      <c r="Q42" s="112"/>
+      <c r="R42" s="112"/>
+      <c r="T42"/>
+      <c r="U42"/>
+    </row>
+    <row r="43" spans="1:26">
+      <c r="A43" s="118"/>
+      <c r="B43" s="170"/>
+      <c r="C43" s="170"/>
+      <c r="D43" s="170"/>
+      <c r="E43" s="170"/>
+      <c r="F43" s="170"/>
+      <c r="G43" s="180"/>
+      <c r="H43" s="112"/>
+      <c r="M43" s="112"/>
+      <c r="N43" s="112"/>
+      <c r="O43" s="112"/>
+      <c r="P43" s="112"/>
+      <c r="Q43" s="112"/>
+      <c r="R43" s="112"/>
+      <c r="T43"/>
+      <c r="U43"/>
+    </row>
+    <row r="44" spans="1:26">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
+    </row>
+    <row r="45" spans="1:26">
+      <c r="A45" s="6"/>
+    </row>
+    <row r="46" spans="1:26">
+      <c r="A46" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="119"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="132"/>
-      <c r="J40" s="132"/>
-      <c r="K40" s="132"/>
-      <c r="L40" s="132"/>
-      <c r="M40" s="37"/>
-      <c r="N40" s="37"/>
-      <c r="O40" s="37"/>
-      <c r="P40" s="37"/>
-      <c r="Q40" s="37"/>
-      <c r="R40" s="37"/>
-      <c r="S40" s="37"/>
-      <c r="T40" s="37"/>
-      <c r="U40" s="38"/>
-      <c r="V40" s="55"/>
-      <c r="W40" s="55"/>
-      <c r="X40" s="55"/>
-      <c r="Y40" s="39"/>
-      <c r="Z40" s="39"/>
-    </row>
-    <row r="41" spans="1:26">
-      <c r="A41" s="186" t="s">
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="119"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="132"/>
+      <c r="J46" s="132"/>
+      <c r="K46" s="132"/>
+      <c r="L46" s="132"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="37"/>
+      <c r="O46" s="37"/>
+      <c r="P46" s="37"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
+      <c r="T46" s="37"/>
+      <c r="U46" s="38"/>
+      <c r="V46" s="132"/>
+      <c r="W46" s="55"/>
+      <c r="X46" s="55"/>
+      <c r="Y46" s="39"/>
+      <c r="Z46" s="39"/>
+    </row>
+    <row r="47" spans="1:26">
+      <c r="A47" s="190" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="186" t="s">
+      <c r="B47" s="190" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="188" t="s">
+      <c r="C47" s="192" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="186" t="s">
+      <c r="D47" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="189" t="s">
+      <c r="E47" s="193" t="s">
         <v>161</v>
       </c>
-      <c r="F41" s="189" t="s">
+      <c r="F47" s="193" t="s">
         <v>176</v>
       </c>
-      <c r="G41" s="186" t="s">
+      <c r="G47" s="190" t="s">
         <v>13</v>
       </c>
-      <c r="H41" s="186" t="s">
+      <c r="H47" s="190" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="193" t="s">
+      <c r="I47" s="197" t="s">
         <v>199</v>
       </c>
-      <c r="J41" s="193" t="s">
+      <c r="J47" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="K41" s="193" t="s">
+      <c r="K47" s="197" t="s">
         <v>201</v>
       </c>
-      <c r="L41" s="196" t="s">
+      <c r="L47" s="186" t="s">
         <v>202</v>
       </c>
-      <c r="M41" s="186" t="s">
+      <c r="M47" s="190" t="s">
         <v>194</v>
       </c>
-      <c r="N41" s="186" t="s">
+      <c r="N47" s="190" t="s">
         <v>208</v>
       </c>
-      <c r="O41" s="188" t="s">
+      <c r="O47" s="192" t="s">
         <v>207</v>
       </c>
-      <c r="P41" s="194" t="s">
+      <c r="P47" s="188" t="s">
         <v>71</v>
       </c>
-      <c r="Q41" s="195"/>
-      <c r="R41" s="194" t="s">
+      <c r="Q47" s="189"/>
+      <c r="R47" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="S41" s="195"/>
-      <c r="T41" s="34" t="s">
+      <c r="S47" s="189"/>
+      <c r="T47" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="U41" s="186" t="s">
+      <c r="U47" s="190" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:26">
-      <c r="A42" s="187"/>
-      <c r="B42" s="187"/>
-      <c r="C42" s="187"/>
-      <c r="D42" s="187"/>
-      <c r="E42" s="190"/>
-      <c r="F42" s="191"/>
-      <c r="G42" s="187"/>
-      <c r="H42" s="187"/>
-      <c r="I42" s="193"/>
-      <c r="J42" s="193"/>
-      <c r="K42" s="193"/>
-      <c r="L42" s="197"/>
-      <c r="M42" s="192"/>
-      <c r="N42" s="192"/>
-      <c r="O42" s="192"/>
-      <c r="P42" s="29" t="s">
+      <c r="V47" s="197" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26">
+      <c r="A48" s="191"/>
+      <c r="B48" s="191"/>
+      <c r="C48" s="191"/>
+      <c r="D48" s="191"/>
+      <c r="E48" s="194"/>
+      <c r="F48" s="195"/>
+      <c r="G48" s="191"/>
+      <c r="H48" s="191"/>
+      <c r="I48" s="197"/>
+      <c r="J48" s="197"/>
+      <c r="K48" s="197"/>
+      <c r="L48" s="187"/>
+      <c r="M48" s="196"/>
+      <c r="N48" s="196"/>
+      <c r="O48" s="196"/>
+      <c r="P48" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="Q42" s="29" t="s">
+      <c r="Q48" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="R42" s="29" t="s">
+      <c r="R48" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="S42" s="29" t="s">
+      <c r="S48" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="T42" s="29" t="s">
+      <c r="T48" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="U42" s="187"/>
-    </row>
-    <row r="43" spans="1:26" ht="30">
-      <c r="A43" s="7">
+      <c r="U48" s="191"/>
+      <c r="V48" s="197"/>
+    </row>
+    <row r="49" spans="1:22" ht="30">
+      <c r="A49" s="7">
         <v>1</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B49" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C49" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="D49" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="120"/>
-      <c r="G43" s="84" t="s">
+      <c r="E49" s="24"/>
+      <c r="F49" s="120"/>
+      <c r="G49" s="84" t="s">
         <v>141</v>
       </c>
-      <c r="H43" s="24"/>
-      <c r="I43" s="133" t="s">
+      <c r="H49" s="24"/>
+      <c r="I49" s="133" t="s">
         <v>203</v>
       </c>
-      <c r="J43" s="133"/>
-      <c r="K43" s="138" t="s">
+      <c r="J49" s="133"/>
+      <c r="K49" s="138" t="s">
         <v>223</v>
       </c>
-      <c r="L43" s="133"/>
-      <c r="M43" s="24" t="s">
+      <c r="L49" s="133"/>
+      <c r="M49" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="N43" s="24" t="s">
+      <c r="N49" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="O43" s="24" t="s">
+      <c r="O49" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="P43" s="24">
+      <c r="P49" s="24">
         <v>0</v>
       </c>
-      <c r="Q43" s="30">
+      <c r="Q49" s="30">
         <v>10</v>
       </c>
-      <c r="R43" s="24"/>
-      <c r="S43" s="30"/>
-      <c r="T43" s="30"/>
-      <c r="U43" s="9"/>
-    </row>
-    <row r="44" spans="1:26">
-      <c r="A44" s="10">
-        <f t="shared" ref="A44:A49" si="0">A43+1</f>
+      <c r="R49" s="24"/>
+      <c r="S49" s="30"/>
+      <c r="T49" s="30"/>
+      <c r="U49" s="9"/>
+      <c r="V49" s="138"/>
+    </row>
+    <row r="50" spans="1:22">
+      <c r="A50" s="10">
+        <f t="shared" ref="A50:A55" si="0">A49+1</f>
         <v>2</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B50" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C50" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="25" t="s">
+      <c r="D50" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="85" t="s">
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="H44" s="25"/>
-      <c r="I44" s="135" t="s">
+      <c r="H50" s="25"/>
+      <c r="I50" s="135" t="s">
         <v>204</v>
       </c>
-      <c r="J44" s="135"/>
-      <c r="K44" s="136" t="s">
+      <c r="J50" s="135"/>
+      <c r="K50" s="136" t="s">
         <v>205</v>
       </c>
-      <c r="L44" s="135"/>
-      <c r="M44" s="25" t="s">
+      <c r="L50" s="135"/>
+      <c r="M50" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="N44" s="25" t="s">
+      <c r="N50" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="O44" s="25" t="s">
+      <c r="O50" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="P44" s="21"/>
-      <c r="Q44" s="31"/>
-      <c r="R44" s="21">
+      <c r="P50" s="21"/>
+      <c r="Q50" s="31"/>
+      <c r="R50" s="21">
         <v>0</v>
       </c>
-      <c r="S44" s="31">
+      <c r="S50" s="31">
         <v>100</v>
       </c>
-      <c r="T44" s="31"/>
-      <c r="U44" s="12"/>
-    </row>
-    <row r="45" spans="1:26">
-      <c r="A45" s="10">
+      <c r="T50" s="31"/>
+      <c r="U50" s="12"/>
+      <c r="V50" s="136" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22">
+      <c r="A51" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B51" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="26" t="s">
+      <c r="C51" s="13"/>
+      <c r="D51" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="86" t="s">
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="86" t="s">
         <v>141</v>
       </c>
-      <c r="H45" s="26" t="b">
+      <c r="H51" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I45" s="135"/>
-      <c r="J45" s="135"/>
-      <c r="K45" s="135"/>
-      <c r="L45" s="135"/>
-      <c r="M45" s="25" t="s">
+      <c r="I51" s="135"/>
+      <c r="J51" s="135"/>
+      <c r="K51" s="135"/>
+      <c r="L51" s="135"/>
+      <c r="M51" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="N45" s="25" t="s">
+      <c r="N51" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="O45" s="25" t="s">
+      <c r="O51" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="P45" s="21"/>
-      <c r="Q45" s="31"/>
-      <c r="R45" s="21"/>
-      <c r="S45" s="31"/>
-      <c r="T45" s="31"/>
-      <c r="U45" s="14"/>
-    </row>
-    <row r="46" spans="1:26">
-      <c r="A46" s="10">
+      <c r="P51" s="21"/>
+      <c r="Q51" s="31"/>
+      <c r="R51" s="21"/>
+      <c r="S51" s="31"/>
+      <c r="T51" s="31"/>
+      <c r="U51" s="14"/>
+      <c r="V51" s="135"/>
+    </row>
+    <row r="52" spans="1:22">
+      <c r="A52" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B52" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="26" t="s">
+      <c r="C52" s="13"/>
+      <c r="D52" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="87"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="135"/>
-      <c r="J46" s="135"/>
-      <c r="K46" s="135"/>
-      <c r="L46" s="135"/>
-      <c r="M46" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="N46" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="O46" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="P46" s="21"/>
-      <c r="Q46" s="31"/>
-      <c r="R46" s="21"/>
-      <c r="S46" s="31"/>
-      <c r="T46" s="31"/>
-      <c r="U46" s="14"/>
-    </row>
-    <row r="47" spans="1:26">
-      <c r="A47" s="10">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="E47" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="F47" s="26"/>
-      <c r="G47" s="86"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="136"/>
-      <c r="J47" s="136"/>
-      <c r="K47" s="136"/>
-      <c r="L47" s="136"/>
-      <c r="M47" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="N47" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="O47" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="P47" s="25"/>
-      <c r="Q47" s="32"/>
-      <c r="R47" s="25"/>
-      <c r="S47" s="32"/>
-      <c r="T47" s="32"/>
-      <c r="U47" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="48" spans="1:26">
-      <c r="A48" s="10">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="86"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="135"/>
-      <c r="J48" s="135"/>
-      <c r="K48" s="135"/>
-      <c r="L48" s="135"/>
-      <c r="M48" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="N48" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="O48" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="P48" s="21"/>
-      <c r="Q48" s="31"/>
-      <c r="R48" s="21"/>
-      <c r="S48" s="31"/>
-      <c r="T48" s="31"/>
-      <c r="U48" s="14"/>
-    </row>
-    <row r="49" spans="1:21">
-      <c r="A49" s="10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="86"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="136"/>
-      <c r="J49" s="136"/>
-      <c r="K49" s="136"/>
-      <c r="L49" s="136"/>
-      <c r="M49" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="N49" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="O49" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="P49" s="21"/>
-      <c r="Q49" s="31"/>
-      <c r="R49" s="21"/>
-      <c r="S49" s="31"/>
-      <c r="T49" s="31"/>
-      <c r="U49" s="14"/>
-    </row>
-    <row r="50" spans="1:21">
-      <c r="A50" s="10"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="86"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="135"/>
-      <c r="J50" s="135"/>
-      <c r="K50" s="135"/>
-      <c r="L50" s="135"/>
-      <c r="M50" s="25"/>
-      <c r="N50" s="25"/>
-      <c r="O50" s="25"/>
-      <c r="P50" s="21"/>
-      <c r="Q50" s="31"/>
-      <c r="R50" s="21"/>
-      <c r="S50" s="31"/>
-      <c r="T50" s="31"/>
-      <c r="U50" s="14"/>
-    </row>
-    <row r="51" spans="1:21">
-      <c r="A51" s="10"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="86"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="136"/>
-      <c r="J51" s="136"/>
-      <c r="K51" s="136"/>
-      <c r="L51" s="136"/>
-      <c r="M51" s="25"/>
-      <c r="N51" s="25"/>
-      <c r="O51" s="25"/>
-      <c r="P51" s="25"/>
-      <c r="Q51" s="32"/>
-      <c r="R51" s="25"/>
-      <c r="S51" s="32"/>
-      <c r="T51" s="32"/>
-      <c r="U51" s="14"/>
-    </row>
-    <row r="52" spans="1:21">
-      <c r="A52" s="10"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="86"/>
-      <c r="H52" s="26"/>
+      <c r="E52" s="82"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="87"/>
+      <c r="H52" s="82"/>
       <c r="I52" s="135"/>
       <c r="J52" s="135"/>
       <c r="K52" s="135"/>
       <c r="L52" s="135"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="25"/>
+      <c r="M52" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="N52" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="O52" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="P52" s="21"/>
       <c r="Q52" s="31"/>
       <c r="R52" s="21"/>
       <c r="S52" s="31"/>
       <c r="T52" s="31"/>
       <c r="U52" s="14"/>
-    </row>
-    <row r="53" spans="1:21">
-      <c r="A53" s="10"/>
-      <c r="B53" s="22"/>
+      <c r="V52" s="135"/>
+    </row>
+    <row r="53" spans="1:22">
+      <c r="A53" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>97</v>
+      </c>
       <c r="C53" s="13"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
+      <c r="D53" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>168</v>
+      </c>
       <c r="F53" s="26"/>
       <c r="G53" s="86"/>
       <c r="H53" s="26"/>
-      <c r="I53" s="135"/>
-      <c r="J53" s="135"/>
-      <c r="K53" s="135"/>
-      <c r="L53" s="135"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="25"/>
-      <c r="P53" s="21"/>
-      <c r="Q53" s="31"/>
-      <c r="R53" s="21"/>
-      <c r="S53" s="31"/>
-      <c r="T53" s="31"/>
-      <c r="U53" s="14"/>
-    </row>
-    <row r="54" spans="1:21">
-      <c r="A54" s="10"/>
-      <c r="B54" s="22"/>
+      <c r="I53" s="136"/>
+      <c r="J53" s="136"/>
+      <c r="K53" s="136"/>
+      <c r="L53" s="136"/>
+      <c r="M53" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="N53" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="O53" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="P53" s="25"/>
+      <c r="Q53" s="32"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="32"/>
+      <c r="T53" s="32"/>
+      <c r="U53" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="V53" s="136"/>
+    </row>
+    <row r="54" spans="1:22">
+      <c r="A54" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>98</v>
+      </c>
       <c r="C54" s="13"/>
-      <c r="D54" s="26"/>
+      <c r="D54" s="26" t="s">
+        <v>113</v>
+      </c>
       <c r="E54" s="26"/>
       <c r="F54" s="26"/>
       <c r="G54" s="86"/>
@@ -6548,40 +6567,61 @@
       <c r="J54" s="135"/>
       <c r="K54" s="135"/>
       <c r="L54" s="135"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="25"/>
+      <c r="M54" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="N54" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="O54" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="P54" s="21"/>
       <c r="Q54" s="31"/>
       <c r="R54" s="21"/>
       <c r="S54" s="31"/>
       <c r="T54" s="31"/>
       <c r="U54" s="14"/>
-    </row>
-    <row r="55" spans="1:21">
-      <c r="A55" s="10"/>
-      <c r="B55" s="22"/>
+      <c r="V54" s="135"/>
+    </row>
+    <row r="55" spans="1:22">
+      <c r="A55" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>115</v>
+      </c>
       <c r="C55" s="13"/>
-      <c r="D55" s="26"/>
+      <c r="D55" s="26" t="s">
+        <v>169</v>
+      </c>
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
       <c r="G55" s="86"/>
       <c r="H55" s="26"/>
-      <c r="I55" s="135"/>
-      <c r="J55" s="135"/>
-      <c r="K55" s="135"/>
-      <c r="L55" s="135"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
+      <c r="I55" s="136"/>
+      <c r="J55" s="136"/>
+      <c r="K55" s="136"/>
+      <c r="L55" s="136"/>
+      <c r="M55" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="N55" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="O55" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="P55" s="21"/>
       <c r="Q55" s="31"/>
       <c r="R55" s="21"/>
       <c r="S55" s="31"/>
       <c r="T55" s="31"/>
       <c r="U55" s="14"/>
-    </row>
-    <row r="56" spans="1:21">
+      <c r="V55" s="136"/>
+    </row>
+    <row r="56" spans="1:22">
       <c r="A56" s="10"/>
       <c r="B56" s="22"/>
       <c r="C56" s="13"/>
@@ -6603,8 +6643,9 @@
       <c r="S56" s="31"/>
       <c r="T56" s="31"/>
       <c r="U56" s="14"/>
-    </row>
-    <row r="57" spans="1:21">
+      <c r="V56" s="135"/>
+    </row>
+    <row r="57" spans="1:22">
       <c r="A57" s="10"/>
       <c r="B57" s="22"/>
       <c r="C57" s="13"/>
@@ -6613,10 +6654,10 @@
       <c r="F57" s="26"/>
       <c r="G57" s="86"/>
       <c r="H57" s="26"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
-      <c r="K57" s="26"/>
-      <c r="L57" s="26"/>
+      <c r="I57" s="136"/>
+      <c r="J57" s="136"/>
+      <c r="K57" s="136"/>
+      <c r="L57" s="136"/>
       <c r="M57" s="25"/>
       <c r="N57" s="25"/>
       <c r="O57" s="25"/>
@@ -6626,8 +6667,9 @@
       <c r="S57" s="32"/>
       <c r="T57" s="32"/>
       <c r="U57" s="14"/>
-    </row>
-    <row r="58" spans="1:21">
+      <c r="V57" s="136"/>
+    </row>
+    <row r="58" spans="1:22">
       <c r="A58" s="10"/>
       <c r="B58" s="22"/>
       <c r="C58" s="13"/>
@@ -6636,10 +6678,10 @@
       <c r="F58" s="26"/>
       <c r="G58" s="86"/>
       <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
-      <c r="K58" s="26"/>
-      <c r="L58" s="26"/>
+      <c r="I58" s="135"/>
+      <c r="J58" s="135"/>
+      <c r="K58" s="135"/>
+      <c r="L58" s="135"/>
       <c r="M58" s="25"/>
       <c r="N58" s="25"/>
       <c r="O58" s="25"/>
@@ -6649,8 +6691,9 @@
       <c r="S58" s="31"/>
       <c r="T58" s="31"/>
       <c r="U58" s="14"/>
-    </row>
-    <row r="59" spans="1:21">
+      <c r="V58" s="135"/>
+    </row>
+    <row r="59" spans="1:22">
       <c r="A59" s="10"/>
       <c r="B59" s="22"/>
       <c r="C59" s="13"/>
@@ -6659,10 +6702,10 @@
       <c r="F59" s="26"/>
       <c r="G59" s="86"/>
       <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="26"/>
-      <c r="K59" s="26"/>
-      <c r="L59" s="26"/>
+      <c r="I59" s="135"/>
+      <c r="J59" s="135"/>
+      <c r="K59" s="135"/>
+      <c r="L59" s="135"/>
       <c r="M59" s="25"/>
       <c r="N59" s="25"/>
       <c r="O59" s="25"/>
@@ -6672,8 +6715,9 @@
       <c r="S59" s="31"/>
       <c r="T59" s="31"/>
       <c r="U59" s="14"/>
-    </row>
-    <row r="60" spans="1:21">
+      <c r="V59" s="135"/>
+    </row>
+    <row r="60" spans="1:22">
       <c r="A60" s="10"/>
       <c r="B60" s="22"/>
       <c r="C60" s="13"/>
@@ -6682,10 +6726,10 @@
       <c r="F60" s="26"/>
       <c r="G60" s="86"/>
       <c r="H60" s="26"/>
-      <c r="I60" s="26"/>
-      <c r="J60" s="26"/>
-      <c r="K60" s="26"/>
-      <c r="L60" s="26"/>
+      <c r="I60" s="135"/>
+      <c r="J60" s="135"/>
+      <c r="K60" s="135"/>
+      <c r="L60" s="135"/>
       <c r="M60" s="25"/>
       <c r="N60" s="25"/>
       <c r="O60" s="25"/>
@@ -6695,8 +6739,9 @@
       <c r="S60" s="31"/>
       <c r="T60" s="31"/>
       <c r="U60" s="14"/>
-    </row>
-    <row r="61" spans="1:21">
+      <c r="V60" s="135"/>
+    </row>
+    <row r="61" spans="1:22">
       <c r="A61" s="10"/>
       <c r="B61" s="22"/>
       <c r="C61" s="13"/>
@@ -6705,10 +6750,10 @@
       <c r="F61" s="26"/>
       <c r="G61" s="86"/>
       <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
-      <c r="K61" s="26"/>
-      <c r="L61" s="26"/>
+      <c r="I61" s="135"/>
+      <c r="J61" s="135"/>
+      <c r="K61" s="135"/>
+      <c r="L61" s="135"/>
       <c r="M61" s="25"/>
       <c r="N61" s="25"/>
       <c r="O61" s="25"/>
@@ -6718,8 +6763,9 @@
       <c r="S61" s="31"/>
       <c r="T61" s="31"/>
       <c r="U61" s="14"/>
-    </row>
-    <row r="62" spans="1:21">
+      <c r="V61" s="135"/>
+    </row>
+    <row r="62" spans="1:22">
       <c r="A62" s="10"/>
       <c r="B62" s="22"/>
       <c r="C62" s="13"/>
@@ -6728,21 +6774,22 @@
       <c r="F62" s="26"/>
       <c r="G62" s="86"/>
       <c r="H62" s="26"/>
-      <c r="I62" s="26"/>
-      <c r="J62" s="26"/>
-      <c r="K62" s="26"/>
-      <c r="L62" s="26"/>
+      <c r="I62" s="135"/>
+      <c r="J62" s="135"/>
+      <c r="K62" s="135"/>
+      <c r="L62" s="135"/>
       <c r="M62" s="25"/>
       <c r="N62" s="25"/>
       <c r="O62" s="25"/>
-      <c r="P62" s="25"/>
-      <c r="Q62" s="32"/>
-      <c r="R62" s="25"/>
-      <c r="S62" s="32"/>
-      <c r="T62" s="32"/>
+      <c r="P62" s="21"/>
+      <c r="Q62" s="31"/>
+      <c r="R62" s="21"/>
+      <c r="S62" s="31"/>
+      <c r="T62" s="31"/>
       <c r="U62" s="14"/>
-    </row>
-    <row r="63" spans="1:21">
+      <c r="V62" s="135"/>
+    </row>
+    <row r="63" spans="1:22">
       <c r="A63" s="10"/>
       <c r="B63" s="22"/>
       <c r="C63" s="13"/>
@@ -6758,14 +6805,15 @@
       <c r="M63" s="25"/>
       <c r="N63" s="25"/>
       <c r="O63" s="25"/>
-      <c r="P63" s="21"/>
-      <c r="Q63" s="31"/>
-      <c r="R63" s="21"/>
-      <c r="S63" s="31"/>
-      <c r="T63" s="31"/>
+      <c r="P63" s="25"/>
+      <c r="Q63" s="32"/>
+      <c r="R63" s="25"/>
+      <c r="S63" s="32"/>
+      <c r="T63" s="32"/>
       <c r="U63" s="14"/>
-    </row>
-    <row r="64" spans="1:21">
+      <c r="V63" s="26"/>
+    </row>
+    <row r="64" spans="1:22">
       <c r="A64" s="10"/>
       <c r="B64" s="22"/>
       <c r="C64" s="13"/>
@@ -6787,8 +6835,9 @@
       <c r="S64" s="31"/>
       <c r="T64" s="31"/>
       <c r="U64" s="14"/>
-    </row>
-    <row r="65" spans="1:21">
+      <c r="V64" s="26"/>
+    </row>
+    <row r="65" spans="1:22">
       <c r="A65" s="10"/>
       <c r="B65" s="22"/>
       <c r="C65" s="13"/>
@@ -6804,48 +6853,206 @@
       <c r="M65" s="25"/>
       <c r="N65" s="25"/>
       <c r="O65" s="25"/>
-      <c r="P65" s="25"/>
-      <c r="Q65" s="32"/>
-      <c r="R65" s="25"/>
-      <c r="S65" s="32"/>
-      <c r="T65" s="32"/>
+      <c r="P65" s="21"/>
+      <c r="Q65" s="31"/>
+      <c r="R65" s="21"/>
+      <c r="S65" s="31"/>
+      <c r="T65" s="31"/>
       <c r="U65" s="14"/>
-    </row>
-    <row r="66" spans="1:21">
-      <c r="A66" s="15"/>
-      <c r="B66" s="23"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="88"/>
-      <c r="H66" s="27"/>
-      <c r="I66" s="27"/>
-      <c r="J66" s="27"/>
-      <c r="K66" s="27"/>
-      <c r="L66" s="27"/>
-      <c r="M66" s="27"/>
-      <c r="N66" s="27"/>
-      <c r="O66" s="27"/>
-      <c r="P66" s="23"/>
-      <c r="Q66" s="33"/>
-      <c r="R66" s="23"/>
-      <c r="S66" s="33"/>
-      <c r="T66" s="33"/>
-      <c r="U66" s="17"/>
+      <c r="V65" s="26"/>
+    </row>
+    <row r="66" spans="1:22">
+      <c r="A66" s="10"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="86"/>
+      <c r="H66" s="26"/>
+      <c r="I66" s="26"/>
+      <c r="J66" s="26"/>
+      <c r="K66" s="26"/>
+      <c r="L66" s="26"/>
+      <c r="M66" s="25"/>
+      <c r="N66" s="25"/>
+      <c r="O66" s="25"/>
+      <c r="P66" s="21"/>
+      <c r="Q66" s="31"/>
+      <c r="R66" s="21"/>
+      <c r="S66" s="31"/>
+      <c r="T66" s="31"/>
+      <c r="U66" s="14"/>
+      <c r="V66" s="26"/>
+    </row>
+    <row r="67" spans="1:22">
+      <c r="A67" s="10"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="86"/>
+      <c r="H67" s="26"/>
+      <c r="I67" s="26"/>
+      <c r="J67" s="26"/>
+      <c r="K67" s="26"/>
+      <c r="L67" s="26"/>
+      <c r="M67" s="25"/>
+      <c r="N67" s="25"/>
+      <c r="O67" s="25"/>
+      <c r="P67" s="21"/>
+      <c r="Q67" s="31"/>
+      <c r="R67" s="21"/>
+      <c r="S67" s="31"/>
+      <c r="T67" s="31"/>
+      <c r="U67" s="14"/>
+      <c r="V67" s="26"/>
+    </row>
+    <row r="68" spans="1:22">
+      <c r="A68" s="10"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="86"/>
+      <c r="H68" s="26"/>
+      <c r="I68" s="26"/>
+      <c r="J68" s="26"/>
+      <c r="K68" s="26"/>
+      <c r="L68" s="26"/>
+      <c r="M68" s="25"/>
+      <c r="N68" s="25"/>
+      <c r="O68" s="25"/>
+      <c r="P68" s="25"/>
+      <c r="Q68" s="32"/>
+      <c r="R68" s="25"/>
+      <c r="S68" s="32"/>
+      <c r="T68" s="32"/>
+      <c r="U68" s="14"/>
+      <c r="V68" s="26"/>
+    </row>
+    <row r="69" spans="1:22">
+      <c r="A69" s="10"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="86"/>
+      <c r="H69" s="26"/>
+      <c r="I69" s="26"/>
+      <c r="J69" s="26"/>
+      <c r="K69" s="26"/>
+      <c r="L69" s="26"/>
+      <c r="M69" s="25"/>
+      <c r="N69" s="25"/>
+      <c r="O69" s="25"/>
+      <c r="P69" s="21"/>
+      <c r="Q69" s="31"/>
+      <c r="R69" s="21"/>
+      <c r="S69" s="31"/>
+      <c r="T69" s="31"/>
+      <c r="U69" s="14"/>
+      <c r="V69" s="26"/>
+    </row>
+    <row r="70" spans="1:22">
+      <c r="A70" s="10"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="86"/>
+      <c r="H70" s="26"/>
+      <c r="I70" s="26"/>
+      <c r="J70" s="26"/>
+      <c r="K70" s="26"/>
+      <c r="L70" s="26"/>
+      <c r="M70" s="25"/>
+      <c r="N70" s="25"/>
+      <c r="O70" s="25"/>
+      <c r="P70" s="21"/>
+      <c r="Q70" s="31"/>
+      <c r="R70" s="21"/>
+      <c r="S70" s="31"/>
+      <c r="T70" s="31"/>
+      <c r="U70" s="14"/>
+      <c r="V70" s="26"/>
+    </row>
+    <row r="71" spans="1:22">
+      <c r="A71" s="10"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="86"/>
+      <c r="H71" s="26"/>
+      <c r="I71" s="26"/>
+      <c r="J71" s="26"/>
+      <c r="K71" s="26"/>
+      <c r="L71" s="26"/>
+      <c r="M71" s="25"/>
+      <c r="N71" s="25"/>
+      <c r="O71" s="25"/>
+      <c r="P71" s="25"/>
+      <c r="Q71" s="32"/>
+      <c r="R71" s="25"/>
+      <c r="S71" s="32"/>
+      <c r="T71" s="32"/>
+      <c r="U71" s="14"/>
+      <c r="V71" s="26"/>
+    </row>
+    <row r="72" spans="1:22">
+      <c r="A72" s="15"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="88"/>
+      <c r="H72" s="27"/>
+      <c r="I72" s="27"/>
+      <c r="J72" s="27"/>
+      <c r="K72" s="27"/>
+      <c r="L72" s="27"/>
+      <c r="M72" s="27"/>
+      <c r="N72" s="27"/>
+      <c r="O72" s="27"/>
+      <c r="P72" s="23"/>
+      <c r="Q72" s="33"/>
+      <c r="R72" s="23"/>
+      <c r="S72" s="33"/>
+      <c r="T72" s="33"/>
+      <c r="U72" s="17"/>
+      <c r="V72" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="L41:L42"/>
+  <mergeCells count="43">
+    <mergeCell ref="V47:V48"/>
+    <mergeCell ref="U47:U48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="O47:O48"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="K47:K48"/>
+    <mergeCell ref="M47:M48"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="N47:N48"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="P47:Q47"/>
     <mergeCell ref="B31:G31"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="B40:G40"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
@@ -6856,23 +7063,17 @@
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="B34:G34"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="U41:U42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="O41:O42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J41:J42"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="R41:S41"/>
-    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
@@ -6882,7 +7083,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{C2D0C7F4-19B0-DB40-AFFD-E6928EE4E5C2}">
       <formula1>isImport</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M43:O66" xr:uid="{1FBC7B49-ABAE-AE4A-8A55-EF1A4EFC4446}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M49:O72" xr:uid="{1FBC7B49-ABAE-AE4A-8A55-EF1A4EFC4446}">
       <formula1>isNullable</formula1>
     </dataValidation>
   </dataValidations>
@@ -6914,7 +7115,7 @@
           <x14:formula1>
             <xm:f>config!$B$5:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G43:G66</xm:sqref>
+          <xm:sqref>G49:G72</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7105,10 +7306,10 @@
         <v>173</v>
       </c>
       <c r="B12" s="122"/>
-      <c r="C12" s="141" t="s">
+      <c r="C12" s="165" t="s">
         <v>174</v>
       </c>
-      <c r="D12" s="141"/>
+      <c r="D12" s="165"/>
       <c r="E12" s="95" t="s">
         <v>175</v>
       </c>
@@ -7123,10 +7324,10 @@
         <v>225</v>
       </c>
       <c r="B13" s="122"/>
-      <c r="C13" s="142" t="s">
+      <c r="C13" s="164" t="s">
         <v>229</v>
       </c>
-      <c r="D13" s="141"/>
+      <c r="D13" s="165"/>
       <c r="E13" s="55" t="s">
         <v>226</v>
       </c>
@@ -7146,10 +7347,10 @@
         <v>176</v>
       </c>
       <c r="B14" s="122"/>
-      <c r="C14" s="141" t="s">
+      <c r="C14" s="165" t="s">
         <v>177</v>
       </c>
-      <c r="D14" s="141"/>
+      <c r="D14" s="165"/>
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="54"/>
@@ -7161,8 +7362,8 @@
         <v>227</v>
       </c>
       <c r="B15" s="122"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="141"/>
+      <c r="C15" s="164"/>
+      <c r="D15" s="165"/>
       <c r="E15" s="55" t="s">
         <v>228</v>
       </c>
@@ -7210,15 +7411,15 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="179" t="s">
+      <c r="A18" s="157" t="s">
         <v>191</v>
       </c>
-      <c r="B18" s="179"/>
-      <c r="C18" s="179"/>
-      <c r="D18" s="179"/>
-      <c r="E18" s="179"/>
-      <c r="F18" s="179"/>
-      <c r="G18" s="179"/>
+      <c r="B18" s="157"/>
+      <c r="C18" s="157"/>
+      <c r="D18" s="157"/>
+      <c r="E18" s="157"/>
+      <c r="F18" s="157"/>
+      <c r="G18" s="157"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -7229,14 +7430,14 @@
       <c r="A19" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="173" t="s">
+      <c r="B19" s="151" t="s">
         <v>182</v>
       </c>
-      <c r="C19" s="174"/>
-      <c r="D19" s="174"/>
-      <c r="E19" s="174"/>
-      <c r="F19" s="174"/>
-      <c r="G19" s="175"/>
+      <c r="C19" s="152"/>
+      <c r="D19" s="152"/>
+      <c r="E19" s="152"/>
+      <c r="F19" s="152"/>
+      <c r="G19" s="153"/>
       <c r="H19" s="105"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -7252,12 +7453,12 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="116"/>
-      <c r="B20" s="157"/>
-      <c r="C20" s="157"/>
-      <c r="D20" s="157"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="157"/>
-      <c r="G20" s="157"/>
+      <c r="B20" s="168"/>
+      <c r="C20" s="168"/>
+      <c r="D20" s="168"/>
+      <c r="E20" s="168"/>
+      <c r="F20" s="168"/>
+      <c r="G20" s="168"/>
       <c r="H20" s="112"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -7272,12 +7473,12 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="117"/>
-      <c r="B21" s="159"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
+      <c r="B21" s="169"/>
+      <c r="C21" s="169"/>
+      <c r="D21" s="169"/>
+      <c r="E21" s="169"/>
+      <c r="F21" s="169"/>
+      <c r="G21" s="169"/>
       <c r="H21" s="112"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -7292,12 +7493,12 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="118"/>
-      <c r="B22" s="161"/>
-      <c r="C22" s="161"/>
-      <c r="D22" s="161"/>
-      <c r="E22" s="161"/>
-      <c r="F22" s="161"/>
-      <c r="G22" s="161"/>
+      <c r="B22" s="170"/>
+      <c r="C22" s="170"/>
+      <c r="D22" s="170"/>
+      <c r="E22" s="170"/>
+      <c r="F22" s="170"/>
+      <c r="G22" s="170"/>
       <c r="H22" s="112"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -7324,15 +7525,15 @@
       <c r="O23" s="112"/>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="176" t="s">
+      <c r="A24" s="154" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="177"/>
-      <c r="C24" s="177"/>
-      <c r="D24" s="177"/>
-      <c r="E24" s="177"/>
-      <c r="F24" s="177"/>
-      <c r="G24" s="178"/>
+      <c r="B24" s="155"/>
+      <c r="C24" s="155"/>
+      <c r="D24" s="155"/>
+      <c r="E24" s="155"/>
+      <c r="F24" s="155"/>
+      <c r="G24" s="156"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -7345,14 +7546,14 @@
       <c r="A25" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="153" t="s">
+      <c r="B25" s="174" t="s">
         <v>183</v>
       </c>
-      <c r="C25" s="153"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="153"/>
-      <c r="F25" s="153"/>
-      <c r="G25" s="153"/>
+      <c r="C25" s="174"/>
+      <c r="D25" s="174"/>
+      <c r="E25" s="174"/>
+      <c r="F25" s="174"/>
+      <c r="G25" s="174"/>
       <c r="H25" s="105"/>
       <c r="M25" s="112"/>
       <c r="N25" s="112"/>
@@ -7368,14 +7569,14 @@
       <c r="A26" s="116">
         <v>1</v>
       </c>
-      <c r="B26" s="154" t="s">
+      <c r="B26" s="175" t="s">
         <v>184</v>
       </c>
-      <c r="C26" s="154"/>
-      <c r="D26" s="154"/>
-      <c r="E26" s="154"/>
-      <c r="F26" s="154"/>
-      <c r="G26" s="154"/>
+      <c r="C26" s="175"/>
+      <c r="D26" s="175"/>
+      <c r="E26" s="175"/>
+      <c r="F26" s="175"/>
+      <c r="G26" s="175"/>
       <c r="H26" s="112"/>
       <c r="I26" s="105"/>
       <c r="J26" s="105"/>
@@ -7390,12 +7591,12 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="117"/>
-      <c r="B27" s="155"/>
-      <c r="C27" s="155"/>
-      <c r="D27" s="155"/>
-      <c r="E27" s="155"/>
-      <c r="F27" s="155"/>
-      <c r="G27" s="155"/>
+      <c r="B27" s="176"/>
+      <c r="C27" s="176"/>
+      <c r="D27" s="176"/>
+      <c r="E27" s="176"/>
+      <c r="F27" s="176"/>
+      <c r="G27" s="176"/>
       <c r="H27" s="112"/>
       <c r="I27" s="105"/>
       <c r="J27" s="105"/>
@@ -7410,12 +7611,12 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="118"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="156"/>
-      <c r="E28" s="156"/>
-      <c r="F28" s="156"/>
-      <c r="G28" s="156"/>
+      <c r="B28" s="177"/>
+      <c r="C28" s="177"/>
+      <c r="D28" s="177"/>
+      <c r="E28" s="177"/>
+      <c r="F28" s="177"/>
+      <c r="G28" s="177"/>
       <c r="H28" s="112"/>
       <c r="I28" s="105"/>
       <c r="J28" s="105"/>
@@ -7454,15 +7655,15 @@
       <c r="T29"/>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="176" t="s">
+      <c r="A30" s="154" t="s">
         <v>193</v>
       </c>
-      <c r="B30" s="177"/>
-      <c r="C30" s="177"/>
-      <c r="D30" s="177"/>
-      <c r="E30" s="177"/>
-      <c r="F30" s="177"/>
-      <c r="G30" s="178"/>
+      <c r="B30" s="155"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="155"/>
+      <c r="G30" s="156"/>
       <c r="M30" s="112"/>
       <c r="N30" s="112"/>
       <c r="O30" s="112"/>
@@ -7471,14 +7672,14 @@
       <c r="A31" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="153" t="s">
+      <c r="B31" s="174" t="s">
         <v>185</v>
       </c>
-      <c r="C31" s="153"/>
-      <c r="D31" s="153"/>
-      <c r="E31" s="153"/>
-      <c r="F31" s="153"/>
-      <c r="G31" s="153"/>
+      <c r="C31" s="174"/>
+      <c r="D31" s="174"/>
+      <c r="E31" s="174"/>
+      <c r="F31" s="174"/>
+      <c r="G31" s="174"/>
       <c r="H31" s="105"/>
       <c r="I31" s="105"/>
       <c r="J31" s="105"/>
@@ -7496,12 +7697,12 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="116"/>
-      <c r="B32" s="157"/>
-      <c r="C32" s="157"/>
-      <c r="D32" s="157"/>
-      <c r="E32" s="157"/>
-      <c r="F32" s="157"/>
-      <c r="G32" s="158"/>
+      <c r="B32" s="168"/>
+      <c r="C32" s="168"/>
+      <c r="D32" s="168"/>
+      <c r="E32" s="168"/>
+      <c r="F32" s="168"/>
+      <c r="G32" s="178"/>
       <c r="H32" s="112"/>
       <c r="I32" s="112"/>
       <c r="J32" s="112"/>
@@ -7519,12 +7720,12 @@
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="117"/>
-      <c r="B33" s="159"/>
-      <c r="C33" s="159"/>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="160"/>
+      <c r="B33" s="169"/>
+      <c r="C33" s="169"/>
+      <c r="D33" s="169"/>
+      <c r="E33" s="169"/>
+      <c r="F33" s="169"/>
+      <c r="G33" s="179"/>
       <c r="H33" s="112"/>
       <c r="I33" s="112"/>
       <c r="J33" s="112"/>
@@ -7539,12 +7740,12 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="118"/>
-      <c r="B34" s="161"/>
-      <c r="C34" s="161"/>
-      <c r="D34" s="161"/>
-      <c r="E34" s="161"/>
-      <c r="F34" s="161"/>
-      <c r="G34" s="162"/>
+      <c r="B34" s="170"/>
+      <c r="C34" s="170"/>
+      <c r="D34" s="170"/>
+      <c r="E34" s="170"/>
+      <c r="F34" s="170"/>
+      <c r="G34" s="180"/>
       <c r="H34" s="112"/>
       <c r="I34" s="112"/>
       <c r="J34" s="112"/>
@@ -7614,84 +7815,84 @@
       <c r="U37" s="58"/>
     </row>
     <row r="38" spans="1:22" ht="30" customHeight="1">
-      <c r="A38" s="189" t="s">
+      <c r="A38" s="193" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="189" t="s">
+      <c r="B38" s="193" t="s">
         <v>119</v>
       </c>
       <c r="C38" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="189" t="s">
+      <c r="D38" s="193" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="189" t="s">
+      <c r="E38" s="193" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="189" t="s">
+      <c r="F38" s="193" t="s">
         <v>176</v>
       </c>
-      <c r="G38" s="189" t="s">
+      <c r="G38" s="193" t="s">
         <v>140</v>
       </c>
-      <c r="H38" s="189" t="s">
+      <c r="H38" s="193" t="s">
         <v>139</v>
       </c>
-      <c r="I38" s="203" t="s">
+      <c r="I38" s="201" t="s">
         <v>199</v>
       </c>
-      <c r="J38" s="205" t="s">
+      <c r="J38" s="203" t="s">
         <v>200</v>
       </c>
-      <c r="K38" s="205" t="s">
+      <c r="K38" s="203" t="s">
         <v>201</v>
       </c>
-      <c r="L38" s="196" t="s">
+      <c r="L38" s="186" t="s">
         <v>202</v>
       </c>
-      <c r="M38" s="186" t="s">
+      <c r="M38" s="190" t="s">
         <v>194</v>
       </c>
-      <c r="N38" s="186" t="s">
+      <c r="N38" s="190" t="s">
         <v>208</v>
       </c>
-      <c r="O38" s="188" t="s">
+      <c r="O38" s="192" t="s">
         <v>207</v>
       </c>
-      <c r="P38" s="202" t="s">
+      <c r="P38" s="199" t="s">
         <v>122</v>
       </c>
       <c r="Q38" s="200"/>
-      <c r="R38" s="199" t="s">
+      <c r="R38" s="205" t="s">
         <v>123</v>
       </c>
       <c r="S38" s="200"/>
       <c r="T38" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U38" s="189" t="s">
+      <c r="U38" s="193" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="15">
-      <c r="A39" s="201"/>
-      <c r="B39" s="201"/>
+      <c r="A39" s="198"/>
+      <c r="B39" s="198"/>
       <c r="C39" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="201"/>
-      <c r="E39" s="191"/>
-      <c r="F39" s="191"/>
-      <c r="G39" s="201"/>
-      <c r="H39" s="201"/>
-      <c r="I39" s="204"/>
-      <c r="J39" s="206"/>
-      <c r="K39" s="206"/>
-      <c r="L39" s="197"/>
-      <c r="M39" s="192"/>
-      <c r="N39" s="192"/>
-      <c r="O39" s="198"/>
+      <c r="D39" s="198"/>
+      <c r="E39" s="195"/>
+      <c r="F39" s="195"/>
+      <c r="G39" s="198"/>
+      <c r="H39" s="198"/>
+      <c r="I39" s="202"/>
+      <c r="J39" s="204"/>
+      <c r="K39" s="204"/>
+      <c r="L39" s="187"/>
+      <c r="M39" s="196"/>
+      <c r="N39" s="196"/>
+      <c r="O39" s="206"/>
       <c r="P39" s="62" t="s">
         <v>126</v>
       </c>
@@ -7707,7 +7908,7 @@
       <c r="T39" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="U39" s="201"/>
+      <c r="U39" s="198"/>
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="64">
@@ -8367,6 +8568,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="U38:U39"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
@@ -8381,28 +8602,8 @@
     <mergeCell ref="J38:J39"/>
     <mergeCell ref="K38:K39"/>
     <mergeCell ref="R38:S38"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B26:G26"/>
     <mergeCell ref="L38:L39"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="B31:G31"/>
     <mergeCell ref="O38:O39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="B34:G34"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">

</xml_diff>